<commit_message>
Update Backlog for Task
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -531,6 +531,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -539,24 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,18 +1183,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,11 +1222,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1235,9 +1235,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1255,10 +1255,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="9" t="s">
         <v>73</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="10" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="G8" s="10">
         <v>10</v>
@@ -1399,9 +1399,11 @@
         <v>0</v>
       </c>
       <c r="I8" s="10">
-        <v>0</v>
-      </c>
-      <c r="J8" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="J8" s="10">
+        <v>4</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1420,7 +1422,7 @@
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="10" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G9" s="10">
         <v>10</v>
@@ -1431,7 +1433,9 @@
       <c r="I9" s="10">
         <v>0</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -1444,7 +1448,7 @@
       <c r="B10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1478,7 +1482,7 @@
       <c r="B11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="16" t="s">
         <v>72</v>
       </c>
@@ -1564,7 +1568,7 @@
       <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="24">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1584,7 +1588,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="13" t="s">
         <v>90</v>
       </c>
@@ -1612,7 +1616,7 @@
       <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="13" t="s">
         <v>91</v>
       </c>
@@ -1640,7 +1644,7 @@
       <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="13" t="s">
         <v>92</v>
       </c>
@@ -1668,7 +1672,7 @@
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="13" t="s">
         <v>93</v>
       </c>
@@ -1696,7 +1700,7 @@
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="14" t="s">
         <v>95</v>
       </c>
@@ -1725,6 +1729,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -1735,15 +1748,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">

</xml_diff>

<commit_message>
Update Backlog and Report 2 part 1.2, 1.3.4.2 and 2.3
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -531,6 +531,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,15 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,18 +1183,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1205,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,11 +1222,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1235,9 +1235,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1255,10 +1255,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="9" t="s">
         <v>73</v>
       </c>
@@ -1436,7 +1436,9 @@
       <c r="J9" s="10">
         <v>1</v>
       </c>
-      <c r="K9" s="10"/>
+      <c r="K9" s="10">
+        <v>3</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
@@ -1448,7 +1450,7 @@
       <c r="B10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="25" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1482,7 +1484,7 @@
       <c r="B11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="16" t="s">
         <v>72</v>
       </c>
@@ -1568,7 +1570,7 @@
       <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="24">
+      <c r="A14" s="18">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1588,7 +1590,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="13" t="s">
         <v>90</v>
       </c>
@@ -1616,7 +1618,7 @@
       <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="13" t="s">
         <v>91</v>
       </c>
@@ -1644,7 +1646,7 @@
       <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="13" t="s">
         <v>92</v>
       </c>
@@ -1672,7 +1674,7 @@
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="13" t="s">
         <v>93</v>
       </c>
@@ -1700,7 +1702,7 @@
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="14" t="s">
         <v>95</v>
       </c>
@@ -1729,15 +1731,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -1748,6 +1741,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">

</xml_diff>

<commit_message>
Update backlog log for task
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -673,6 +673,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -682,23 +700,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -732,12 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,7 +799,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,7 +834,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1364,18 +1364,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1386,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,11 +1403,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1416,9 +1416,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1436,10 +1436,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="9" t="s">
         <v>73</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="B10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="28" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="22" t="s">
@@ -1717,7 +1717,7 @@
       <c r="B11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="22" t="s">
         <v>72</v>
       </c>
@@ -1831,7 +1831,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="24">
+      <c r="A14" s="30">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1851,7 +1851,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="13" t="s">
         <v>90</v>
       </c>
@@ -1889,7 +1889,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="13" t="s">
         <v>91</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="13" t="s">
         <v>92</v>
       </c>
@@ -1965,7 +1965,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="13" t="s">
         <v>93</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="14" t="s">
         <v>95</v>
       </c>
@@ -2042,6 +2042,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2052,15 +2061,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,11 +2093,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2106,9 +2106,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2126,10 +2126,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="9" t="s">
         <v>73</v>
       </c>
@@ -2159,7 +2159,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
+      <c r="A5" s="30">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2179,19 +2179,19 @@
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="35">
         <v>4</v>
       </c>
       <c r="H6" s="10"/>
@@ -2203,15 +2203,15 @@
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="10" t="s">
         <v>102</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="34"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -2221,15 +2221,15 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="35"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -2239,7 +2239,7 @@
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="10" t="s">
         <v>104</v>
       </c>
@@ -2265,19 +2265,19 @@
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="10" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="35">
         <v>4</v>
       </c>
       <c r="H10" s="10"/>
@@ -2289,17 +2289,17 @@
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="35"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -2309,7 +2309,7 @@
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="6" t="s">
         <v>116</v>
       </c>
@@ -2347,12 +2347,14 @@
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="10" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="G13" s="20">
         <v>2</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="10">
+        <v>2</v>
+      </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -2370,10 +2372,10 @@
       <c r="C14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="45"/>
+      <c r="E14" s="34"/>
       <c r="F14" s="15" t="s">
         <v>66</v>
       </c>
@@ -2542,15 +2544,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="D10:E11"/>
@@ -2561,6 +2554,15 @@
     <mergeCell ref="D6:E8"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="F6:F8"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F6 F9:F20">

</xml_diff>

<commit_message>
Update My name in backlog(TuanLD -> TuanLT) :))
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -229,9 +229,6 @@
     <t>DuyPK</t>
   </si>
   <si>
-    <t>TuanLD</t>
-  </si>
-  <si>
     <t>ThinhLT</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>Not complete in sprint 1</t>
+  </si>
+  <si>
+    <t>TuanLT</t>
   </si>
 </sst>
 </file>
@@ -673,6 +673,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,52 +701,43 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,18 +1364,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1386,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,11 +1403,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1416,9 +1416,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1436,36 +1436,36 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -1476,14 +1476,14 @@
         <v>63</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G5" s="10">
         <v>10</v>
@@ -1518,14 +1518,14 @@
         <v>64</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="10">
         <v>5</v>
@@ -1557,7 +1557,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="22" t="s">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="E7" s="23"/>
       <c r="F7" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="10">
         <v>10</v>
@@ -1593,15 +1593,15 @@
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="22" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="10">
         <v>10</v>
@@ -1637,11 +1637,11 @@
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="22" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="10">
         <v>10</v>
@@ -1673,17 +1673,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="10">
         <v>10</v>
@@ -1715,15 +1715,15 @@
         <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="29"/>
+        <v>74</v>
+      </c>
+      <c r="C11" s="32"/>
       <c r="D11" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="10">
         <v>20</v>
@@ -1755,15 +1755,15 @@
         <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="22" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="10">
         <v>2</v>
@@ -1795,15 +1795,15 @@
         <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G13" s="10">
         <v>2</v>
@@ -1831,11 +1831,11 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="24">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="22"/>
@@ -1851,17 +1851,17 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="22" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" s="10">
         <v>4</v>
@@ -1889,9 +1889,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="22" t="s">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G16" s="10">
         <v>4</v>
@@ -1927,17 +1927,17 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G17" s="10">
         <v>4</v>
@@ -1965,17 +1965,17 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -2003,17 +2003,17 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="10">
         <v>2</v>
@@ -2042,15 +2042,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2061,6 +2052,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,11 +2093,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="A1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2106,14 +2106,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2126,44 +2126,44 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="24">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="22"/>
@@ -2179,19 +2179,19 @@
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="28" t="s">
+      <c r="D6" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="33">
         <v>4</v>
       </c>
       <c r="H6" s="10"/>
@@ -2203,15 +2203,15 @@
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="36"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -2221,15 +2221,15 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -2239,19 +2239,19 @@
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="10">
         <v>10</v>
@@ -2265,19 +2265,19 @@
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="39"/>
+      <c r="D10" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="37"/>
       <c r="F10" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="33">
         <v>4</v>
       </c>
       <c r="H10" s="10"/>
@@ -2289,17 +2289,17 @@
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -2309,13 +2309,13 @@
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="15" t="s">
@@ -2337,17 +2337,17 @@
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G13" s="20">
         <v>2</v>
@@ -2367,15 +2367,15 @@
         <v>2</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="15" t="s">
         <v>66</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="22" t="s">
@@ -2421,11 +2421,11 @@
         <v>4</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="15" t="s">
@@ -2447,13 +2447,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>114</v>
-      </c>
       <c r="D17" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="15" t="s">
@@ -2475,10 +2475,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>68</v>
@@ -2503,13 +2503,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="15" t="s">
@@ -2544,6 +2544,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="D10:E11"/>
@@ -2554,15 +2563,6 @@
     <mergeCell ref="D6:E8"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F6 F9:F20">
@@ -2594,17 +2594,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performance Point Day 4
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -447,17 +447,17 @@
     <t>Wait for approve</t>
   </si>
   <si>
-    <t>Not meet the deadline</t>
-  </si>
-  <si>
     <t>Not working on it</t>
   </si>
   <si>
-    <t>In time:
-Not meet the demand</t>
+    <t>In time</t>
   </si>
   <si>
     <t>Design site page builder</t>
+  </si>
+  <si>
+    <t>Not meet the deadline:
+lack of some enities, confuse about entity relation</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1044,6 +1044,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,7 +1111,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1140,7 +1146,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2382,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,7 +2891,7 @@
       <c r="D21" s="93"/>
       <c r="E21" s="94"/>
       <c r="F21" s="41" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G21" s="39">
         <v>2</v>
@@ -2895,36 +2901,34 @@
       <c r="J21" s="39">
         <v>1.5</v>
       </c>
-      <c r="K21" s="40">
-        <v>1</v>
-      </c>
+      <c r="K21" s="40"/>
       <c r="L21" s="40"/>
       <c r="M21" s="40"/>
       <c r="N21" s="41"/>
     </row>
-    <row r="22" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
+    <row r="22" spans="1:14" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
         <v>19</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="93"/>
       <c r="E22" s="94"/>
-      <c r="F22" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="39">
-        <v>2</v>
-      </c>
-      <c r="H22" s="39"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="41"/>
+      <c r="F22" s="109" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="44">
+        <v>2</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="108"/>
+      <c r="L22" s="108"/>
+      <c r="M22" s="108"/>
+      <c r="N22" s="109"/>
     </row>
     <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
@@ -3185,7 +3189,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3224,7 +3228,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="103" t="s">
         <v>132</v>
       </c>
@@ -3234,10 +3238,12 @@
       <c r="C4" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="51" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="51"/>
+      <c r="D4" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="51">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="103"/>
@@ -3246,24 +3252,26 @@
         <v>137</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="104"/>
       <c r="B6" s="52" t="s">
         <v>108</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="51"/>
+        <v>141</v>
+      </c>
+      <c r="E6" s="51">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="104"/>
@@ -3274,7 +3282,7 @@
         <v>137</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="51">
         <v>0</v>

</xml_diff>

<commit_message>
Performance Point Day 5
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -441,9 +441,6 @@
     <t>Design</t>
   </si>
   <si>
-    <t>Physical DB</t>
-  </si>
-  <si>
     <t>Wait for approve</t>
   </si>
   <si>
@@ -456,8 +453,17 @@
     <t>Design site page builder</t>
   </si>
   <si>
+    <t>Not meet the deadline.
+Delay 1 former task 
+Not fill in the backlog</t>
+  </si>
+  <si>
+    <t>In time
+Need more focus to complete assigned  task</t>
+  </si>
+  <si>
     <t>Not meet the deadline:
-lack of some enities, confuse about entity relation</t>
+Lack of some enities, confuse about entity relation</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -873,193 +879,196 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1424,10 +1433,10 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="57" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1441,8 +1450,8 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1454,8 +1463,8 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1467,7 +1476,7 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1482,10 +1491,10 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="57" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1499,8 +1508,8 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1529,10 +1538,10 @@
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="57" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1546,8 +1555,8 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1559,8 +1568,8 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="5" t="s">
         <v>49</v>
       </c>
@@ -1572,10 +1581,10 @@
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="57" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1589,8 +1598,8 @@
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1602,8 +1611,8 @@
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1615,8 +1624,8 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
@@ -1628,10 +1637,10 @@
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1645,8 +1654,8 @@
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1658,10 +1667,10 @@
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="57" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1675,8 +1684,8 @@
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1686,18 +1695,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1725,11 +1734,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1738,9 +1747,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1758,10 +1767,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -1800,10 +1809,10 @@
       <c r="C5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="57"/>
+      <c r="E5" s="59"/>
       <c r="F5" s="10" t="s">
         <v>92</v>
       </c>
@@ -1842,10 +1851,10 @@
       <c r="C6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="10" t="s">
         <v>92</v>
       </c>
@@ -1882,10 +1891,10 @@
         <v>95</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="57"/>
+      <c r="E7" s="59"/>
       <c r="F7" s="10" t="s">
         <v>92</v>
       </c>
@@ -1918,10 +1927,10 @@
         <v>94</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="57"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="10" t="s">
         <v>92</v>
       </c>
@@ -1958,10 +1967,10 @@
         <v>65</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="57"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="10" t="s">
         <v>92</v>
       </c>
@@ -1997,13 +2006,13 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="57"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="10" t="s">
         <v>92</v>
       </c>
@@ -2039,11 +2048,11 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="56" t="s">
+      <c r="C11" s="65"/>
+      <c r="D11" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="57"/>
+      <c r="E11" s="59"/>
       <c r="F11" s="10" t="s">
         <v>92</v>
       </c>
@@ -2080,10 +2089,10 @@
         <v>85</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="57"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="10" t="s">
         <v>76</v>
       </c>
@@ -2120,10 +2129,10 @@
         <v>86</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="57"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="10" t="s">
         <v>92</v>
       </c>
@@ -2153,15 +2162,15 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="58">
+      <c r="A14" s="66">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -2173,15 +2182,15 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="57"/>
+      <c r="E15" s="59"/>
       <c r="F15" s="10" t="s">
         <v>92</v>
       </c>
@@ -2211,15 +2220,15 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="57"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="10" t="s">
         <v>92</v>
       </c>
@@ -2249,15 +2258,15 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="57"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="10" t="s">
         <v>92</v>
       </c>
@@ -2287,15 +2296,15 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="57"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="10" t="s">
         <v>92</v>
       </c>
@@ -2325,15 +2334,15 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="60"/>
+      <c r="A19" s="68"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="57"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="10" t="s">
         <v>92</v>
       </c>
@@ -2364,6 +2373,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2374,15 +2392,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2398,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,11 +2424,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2428,9 +2437,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2448,10 +2457,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2490,10 +2499,10 @@
       <c r="C5" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="44" t="s">
         <v>92</v>
       </c>
@@ -2517,12 +2526,12 @@
       <c r="B6" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="110" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="111"/>
-      <c r="F6" s="54" t="s">
+      <c r="E6" s="79"/>
+      <c r="F6" s="52" t="s">
         <v>92</v>
       </c>
       <c r="G6" s="44">
@@ -2549,10 +2558,10 @@
       <c r="B7" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="54" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="52" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="44">
@@ -2897,10 +2906,10 @@
       <c r="B21" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="53"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="96"/>
       <c r="E21" s="97"/>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="52" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="44">
@@ -2911,10 +2920,10 @@
       <c r="J21" s="44">
         <v>1.5</v>
       </c>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="54"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
@@ -2972,10 +2981,10 @@
         <v>119</v>
       </c>
       <c r="C24" s="26"/>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="76"/>
+      <c r="E24" s="105"/>
       <c r="F24" s="27" t="s">
         <v>76</v>
       </c>
@@ -2995,15 +3004,15 @@
       <c r="N24" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="58">
+      <c r="A43" s="66">
         <v>1</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>98</v>
       </c>
       <c r="C43" s="11"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="57"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="10"/>
       <c r="G43" s="17"/>
       <c r="H43" s="10"/>
@@ -3015,19 +3024,19 @@
       <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
+      <c r="A44" s="67"/>
       <c r="B44" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="70" t="s">
+      <c r="D44" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="71"/>
-      <c r="F44" s="65" t="s">
+      <c r="E44" s="70"/>
+      <c r="F44" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="67">
+      <c r="G44" s="100">
         <v>4</v>
       </c>
       <c r="H44" s="10"/>
@@ -3039,15 +3048,15 @@
       <c r="N44" s="10"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="77"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="68"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="103"/>
+      <c r="G45" s="101"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -3057,15 +3066,15 @@
       <c r="N45" s="10"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
+      <c r="A46" s="67"/>
       <c r="B46" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="66"/>
-      <c r="G46" s="69"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="102"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
@@ -3075,17 +3084,17 @@
       <c r="N46" s="10"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
+      <c r="A47" s="67"/>
       <c r="B47" s="10" t="s">
         <v>102</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="56" t="s">
+      <c r="D47" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="57"/>
+      <c r="E47" s="59"/>
       <c r="F47" s="15" t="s">
         <v>76</v>
       </c>
@@ -3101,19 +3110,19 @@
       <c r="N47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
+      <c r="A48" s="67"/>
       <c r="B48" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="70" t="s">
+      <c r="D48" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="71"/>
+      <c r="E48" s="70"/>
       <c r="F48" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="67">
+      <c r="G48" s="100">
         <v>4</v>
       </c>
       <c r="H48" s="10"/>
@@ -3125,17 +3134,17 @@
       <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="59"/>
+      <c r="A49" s="67"/>
       <c r="B49" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="73"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="74"/>
       <c r="F49" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="69"/>
+      <c r="G49" s="102"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
@@ -3145,15 +3154,15 @@
       <c r="N49" s="10"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
+      <c r="A50" s="75"/>
       <c r="B50" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="56" t="s">
+      <c r="D50" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="57"/>
+      <c r="E50" s="59"/>
       <c r="F50" s="15" t="s">
         <v>66</v>
       </c>
@@ -3170,6 +3179,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D4:E4"/>
@@ -3182,11 +3196,6 @@
     <mergeCell ref="D8:E11"/>
     <mergeCell ref="D12:E16"/>
     <mergeCell ref="D17:E23"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:F44 F47:F50 F5:F24">
@@ -3200,10 +3209,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3217,13 +3226,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
@@ -3243,188 +3252,190 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="107"/>
+      <c r="B6" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="107"/>
+      <c r="B7" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="109" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="113" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="114" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="110"/>
+      <c r="B9" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="113" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="107">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="107" t="s">
+      <c r="E9" s="50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="110"/>
+      <c r="B10" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="107" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="106"/>
-      <c r="B6" s="109" t="s">
+      <c r="D10" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="111" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="49"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="112"/>
+      <c r="B12" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="107" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="108" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="107">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="106"/>
-      <c r="B7" s="109" t="s">
+      <c r="C12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="49"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="112"/>
+      <c r="B13" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C13" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="107" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="100" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="101" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C14" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="101"/>
-      <c r="B10" s="52" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="112"/>
+      <c r="B15" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C15" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="101"/>
-      <c r="B11" s="52" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="49"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="112"/>
+      <c r="B16" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C16" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="103" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="103" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="49"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3456,7 +3467,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Performance Point Day 5
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -448,9 +448,6 @@
   </si>
   <si>
     <t>In time</t>
-  </si>
-  <si>
-    <t>Design site page builder</t>
   </si>
   <si>
     <t>Not meet the deadline.
@@ -458,12 +455,13 @@
 Not fill in the backlog</t>
   </si>
   <si>
-    <t>In time
-Need more focus to complete assigned  task</t>
-  </si>
-  <si>
     <t>Not meet the deadline:
 Lack of some enities, confuse about entity relation</t>
+  </si>
+  <si>
+    <t>Not meet the deadline.
+Missing some relative page
+Need more focus to complete assigned  task</t>
   </si>
 </sst>
 </file>
@@ -734,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -878,8 +876,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -892,10 +888,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -905,6 +906,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -924,13 +934,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -938,18 +948,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1025,24 +1044,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,12 +1064,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1433,10 +1428,10 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="56" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1450,8 +1445,8 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1463,8 +1458,8 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1471,7 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1491,10 +1486,10 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1508,8 +1503,8 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="5" t="s">
         <v>46</v>
       </c>
@@ -1538,10 +1533,10 @@
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1555,8 +1550,8 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1568,8 +1563,8 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="5" t="s">
         <v>49</v>
       </c>
@@ -1581,10 +1576,10 @@
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="56" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1598,8 +1593,8 @@
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1611,8 +1606,8 @@
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1624,8 +1619,8 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
@@ -1637,10 +1632,10 @@
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1654,8 +1649,8 @@
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1667,10 +1662,10 @@
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="56" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1684,8 +1679,8 @@
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1695,18 +1690,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1734,11 +1729,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1747,9 +1742,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1767,10 +1762,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -1809,10 +1804,10 @@
       <c r="C5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="59"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="10" t="s">
         <v>92</v>
       </c>
@@ -1851,10 +1846,10 @@
       <c r="C6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="59"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="10" t="s">
         <v>92</v>
       </c>
@@ -1891,10 +1886,10 @@
         <v>95</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="59"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="10" t="s">
         <v>92</v>
       </c>
@@ -1927,10 +1922,10 @@
         <v>94</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="59"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="10" t="s">
         <v>92</v>
       </c>
@@ -1967,10 +1962,10 @@
         <v>65</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="59"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="10" t="s">
         <v>92</v>
       </c>
@@ -2006,13 +2001,13 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="59"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="10" t="s">
         <v>92</v>
       </c>
@@ -2048,11 +2043,11 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="58" t="s">
+      <c r="C11" s="67"/>
+      <c r="D11" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="59"/>
+      <c r="E11" s="58"/>
       <c r="F11" s="10" t="s">
         <v>92</v>
       </c>
@@ -2089,10 +2084,10 @@
         <v>85</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="59"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="10" t="s">
         <v>76</v>
       </c>
@@ -2129,10 +2124,10 @@
         <v>86</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="59"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="10" t="s">
         <v>92</v>
       </c>
@@ -2162,15 +2157,15 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="66">
+      <c r="A14" s="59">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -2182,15 +2177,15 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="59"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="10" t="s">
         <v>92</v>
       </c>
@@ -2220,15 +2215,15 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="59"/>
+      <c r="E16" s="58"/>
       <c r="F16" s="10" t="s">
         <v>92</v>
       </c>
@@ -2258,15 +2253,15 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="67"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="10" t="s">
         <v>92</v>
       </c>
@@ -2296,15 +2291,15 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="59"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="10" t="s">
         <v>92</v>
       </c>
@@ -2334,15 +2329,15 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="59"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="10" t="s">
         <v>92</v>
       </c>
@@ -2373,15 +2368,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2392,6 +2378,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2407,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,11 +2419,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2437,9 +2432,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2457,10 +2452,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2499,10 +2494,10 @@
       <c r="C5" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="77"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="44" t="s">
         <v>92</v>
       </c>
@@ -2526,12 +2521,12 @@
       <c r="B6" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="78" t="s">
+      <c r="C6" s="49"/>
+      <c r="D6" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="52" t="s">
+      <c r="E6" s="84"/>
+      <c r="F6" s="50" t="s">
         <v>92</v>
       </c>
       <c r="G6" s="44">
@@ -2558,10 +2553,10 @@
       <c r="B7" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="52" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="50" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="44">
@@ -2589,10 +2584,10 @@
         <v>109</v>
       </c>
       <c r="C8" s="21"/>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="83"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="22" t="s">
         <v>66</v>
       </c>
@@ -2615,8 +2610,8 @@
         <v>111</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="85"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="90"/>
       <c r="F9" s="22" t="s">
         <v>66</v>
       </c>
@@ -2639,8 +2634,8 @@
         <v>112</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90"/>
       <c r="F10" s="22" t="s">
         <v>66</v>
       </c>
@@ -2663,8 +2658,8 @@
         <v>113</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="87"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="22" t="s">
         <v>66</v>
       </c>
@@ -2687,10 +2682,10 @@
         <v>110</v>
       </c>
       <c r="C12" s="31"/>
-      <c r="D12" s="88" t="s">
+      <c r="D12" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="89"/>
+      <c r="E12" s="94"/>
       <c r="F12" s="32" t="s">
         <v>66</v>
       </c>
@@ -2713,8 +2708,8 @@
         <v>114</v>
       </c>
       <c r="C13" s="33"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="32" t="s">
         <v>66</v>
       </c>
@@ -2737,8 +2732,8 @@
         <v>126</v>
       </c>
       <c r="C14" s="33"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="91"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
       <c r="F14" s="32" t="s">
         <v>66</v>
       </c>
@@ -2761,8 +2756,8 @@
         <v>115</v>
       </c>
       <c r="C15" s="37"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="91"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
       <c r="F15" s="32" t="s">
         <v>66</v>
       </c>
@@ -2785,8 +2780,8 @@
         <v>116</v>
       </c>
       <c r="C16" s="37"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="98"/>
       <c r="F16" s="32" t="s">
         <v>66</v>
       </c>
@@ -2809,10 +2804,10 @@
         <v>127</v>
       </c>
       <c r="C17" s="40"/>
-      <c r="D17" s="94" t="s">
+      <c r="D17" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="95"/>
+      <c r="E17" s="100"/>
       <c r="F17" s="41" t="s">
         <v>76</v>
       </c>
@@ -2835,8 +2830,8 @@
         <v>122</v>
       </c>
       <c r="C18" s="40"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="102"/>
       <c r="F18" s="41" t="s">
         <v>66</v>
       </c>
@@ -2859,8 +2854,8 @@
         <v>123</v>
       </c>
       <c r="C19" s="40"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="102"/>
       <c r="F19" s="41" t="s">
         <v>66</v>
       </c>
@@ -2883,8 +2878,8 @@
         <v>124</v>
       </c>
       <c r="C20" s="40"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="97"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="102"/>
       <c r="F20" s="41" t="s">
         <v>66</v>
       </c>
@@ -2906,10 +2901,10 @@
       <c r="B21" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="52" t="s">
+      <c r="C21" s="49"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="50" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="44">
@@ -2920,10 +2915,10 @@
       <c r="J21" s="44">
         <v>1.5</v>
       </c>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
     </row>
     <row r="22" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
@@ -2933,8 +2928,8 @@
         <v>118</v>
       </c>
       <c r="C22" s="40"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="97"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="102"/>
       <c r="F22" s="41" t="s">
         <v>76</v>
       </c>
@@ -2957,8 +2952,8 @@
         <v>125</v>
       </c>
       <c r="C23" s="40"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="99"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="104"/>
       <c r="F23" s="41" t="s">
         <v>66</v>
       </c>
@@ -2981,10 +2976,10 @@
         <v>119</v>
       </c>
       <c r="C24" s="26"/>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="105"/>
+      <c r="E24" s="77"/>
       <c r="F24" s="27" t="s">
         <v>76</v>
       </c>
@@ -3004,15 +2999,15 @@
       <c r="N24" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="66">
+      <c r="A43" s="59">
         <v>1</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>98</v>
       </c>
       <c r="C43" s="11"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="10"/>
       <c r="G43" s="17"/>
       <c r="H43" s="10"/>
@@ -3024,19 +3019,19 @@
       <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="67"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="69" t="s">
+      <c r="D44" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="70"/>
-      <c r="F44" s="64" t="s">
+      <c r="E44" s="72"/>
+      <c r="F44" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="100">
+      <c r="G44" s="68">
         <v>4</v>
       </c>
       <c r="H44" s="10"/>
@@ -3048,15 +3043,15 @@
       <c r="N44" s="10"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="67"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="71"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="103"/>
-      <c r="G45" s="101"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -3066,15 +3061,15 @@
       <c r="N45" s="10"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="67"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="73"/>
       <c r="E46" s="74"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="102"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="70"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
@@ -3084,17 +3079,17 @@
       <c r="N46" s="10"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="67"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="10" t="s">
         <v>102</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="58" t="s">
+      <c r="D47" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="59"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="15" t="s">
         <v>76</v>
       </c>
@@ -3110,19 +3105,19 @@
       <c r="N47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="67"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="69" t="s">
+      <c r="D48" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="70"/>
+      <c r="E48" s="72"/>
       <c r="F48" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="100">
+      <c r="G48" s="68">
         <v>4</v>
       </c>
       <c r="H48" s="10"/>
@@ -3134,7 +3129,7 @@
       <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="67"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="10" t="s">
         <v>97</v>
       </c>
@@ -3144,7 +3139,7 @@
       <c r="F49" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="102"/>
+      <c r="G49" s="70"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
@@ -3154,15 +3149,15 @@
       <c r="N49" s="10"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="75"/>
+      <c r="A50" s="80"/>
       <c r="B50" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="58" t="s">
+      <c r="D50" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="59"/>
+      <c r="E50" s="58"/>
       <c r="F50" s="15" t="s">
         <v>66</v>
       </c>
@@ -3179,11 +3174,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D4:E4"/>
@@ -3196,6 +3186,11 @@
     <mergeCell ref="D8:E11"/>
     <mergeCell ref="D12:E16"/>
     <mergeCell ref="D17:E23"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:F44 F47:F50 F5:F24">
@@ -3212,7 +3207,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3226,13 +3221,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
@@ -3252,53 +3247,53 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="106" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="55">
+      <c r="D4" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="106"/>
-      <c r="B5" s="107"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="44" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="107"/>
-      <c r="B6" s="56" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="53" t="s">
         <v>108</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="44">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="107"/>
-      <c r="B7" s="56" t="s">
+      <c r="A7" s="106"/>
+      <c r="B7" s="53" t="s">
         <v>68</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -3307,126 +3302,126 @@
       <c r="D7" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="114" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="110"/>
-      <c r="B9" s="53" t="s">
+      <c r="D8" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="109"/>
+      <c r="B9" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="109"/>
+      <c r="B10" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="114" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="50">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="110"/>
-      <c r="B10" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="113" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="113" t="s">
+      <c r="D10" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="110" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="52" t="s">
         <v>69</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="49"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="112"/>
-      <c r="B12" s="54" t="s">
+      <c r="A12" s="111"/>
+      <c r="B12" s="52" t="s">
         <v>108</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="49"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="112"/>
-      <c r="B13" s="54" t="s">
+      <c r="A13" s="111"/>
+      <c r="B13" s="52" t="s">
         <v>68</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="49"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="110" t="s">
         <v>134</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="52" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="49"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="112"/>
-      <c r="B15" s="54" t="s">
+      <c r="A15" s="111"/>
+      <c r="B15" s="52" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="49"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="112"/>
-      <c r="B16" s="54" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="52" t="s">
         <v>68</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>137</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="49"/>
+      <c r="E16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add AddProduct Page, update Backlog
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -906,6 +906,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -915,23 +933,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -942,18 +1035,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -961,87 +1042,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,7 +1125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1160,7 +1160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1690,18 +1690,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1729,11 +1729,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1742,9 +1742,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1762,10 +1762,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="65"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="63" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="57" t="s">
@@ -2043,7 +2043,7 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="57" t="s">
         <v>71</v>
       </c>
@@ -2157,7 +2157,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="59">
+      <c r="A14" s="65">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2177,7 +2177,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="60"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -2329,7 +2329,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="67"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -2368,6 +2368,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2378,15 +2387,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2419,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2432,9 +2432,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2452,10 +2452,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="65"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2494,10 +2494,10 @@
       <c r="C5" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="82"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="44" t="s">
         <v>92</v>
       </c>
@@ -2522,10 +2522,10 @@
         <v>120</v>
       </c>
       <c r="C6" s="49"/>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="84"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="50" t="s">
         <v>92</v>
       </c>
@@ -2554,8 +2554,8 @@
         <v>121</v>
       </c>
       <c r="C7" s="49"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="80"/>
       <c r="F7" s="50" t="s">
         <v>92</v>
       </c>
@@ -2584,10 +2584,10 @@
         <v>109</v>
       </c>
       <c r="C8" s="21"/>
-      <c r="D8" s="87" t="s">
+      <c r="D8" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="88"/>
+      <c r="E8" s="82"/>
       <c r="F8" s="22" t="s">
         <v>66</v>
       </c>
@@ -2610,8 +2610,8 @@
         <v>111</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="90"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="22" t="s">
         <v>66</v>
       </c>
@@ -2634,8 +2634,8 @@
         <v>112</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="90"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="84"/>
       <c r="F10" s="22" t="s">
         <v>66</v>
       </c>
@@ -2658,8 +2658,8 @@
         <v>113</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="92"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="22" t="s">
         <v>66</v>
       </c>
@@ -2682,10 +2682,10 @@
         <v>110</v>
       </c>
       <c r="C12" s="31"/>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="94"/>
+      <c r="E12" s="88"/>
       <c r="F12" s="32" t="s">
         <v>66</v>
       </c>
@@ -2708,8 +2708,8 @@
         <v>114</v>
       </c>
       <c r="C13" s="33"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="96"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90"/>
       <c r="F13" s="32" t="s">
         <v>66</v>
       </c>
@@ -2732,8 +2732,8 @@
         <v>126</v>
       </c>
       <c r="C14" s="33"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="96"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="90"/>
       <c r="F14" s="32" t="s">
         <v>66</v>
       </c>
@@ -2756,8 +2756,8 @@
         <v>115</v>
       </c>
       <c r="C15" s="37"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="96"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="32" t="s">
         <v>66</v>
       </c>
@@ -2780,8 +2780,8 @@
         <v>116</v>
       </c>
       <c r="C16" s="37"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="98"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="92"/>
       <c r="F16" s="32" t="s">
         <v>66</v>
       </c>
@@ -2804,10 +2804,10 @@
         <v>127</v>
       </c>
       <c r="C17" s="40"/>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="100"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="41" t="s">
         <v>76</v>
       </c>
@@ -2830,10 +2830,10 @@
         <v>122</v>
       </c>
       <c r="C18" s="40"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="102"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
       <c r="F18" s="41" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G18" s="39">
         <v>2</v>
@@ -2854,8 +2854,8 @@
         <v>123</v>
       </c>
       <c r="C19" s="40"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="102"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="96"/>
       <c r="F19" s="41" t="s">
         <v>66</v>
       </c>
@@ -2878,8 +2878,8 @@
         <v>124</v>
       </c>
       <c r="C20" s="40"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="102"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
       <c r="F20" s="41" t="s">
         <v>66</v>
       </c>
@@ -2902,8 +2902,8 @@
         <v>117</v>
       </c>
       <c r="C21" s="49"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="102"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
       <c r="F21" s="50" t="s">
         <v>92</v>
       </c>
@@ -2915,7 +2915,9 @@
       <c r="J21" s="44">
         <v>1.5</v>
       </c>
-      <c r="K21" s="49"/>
+      <c r="K21" s="49">
+        <v>2</v>
+      </c>
       <c r="L21" s="49"/>
       <c r="M21" s="49"/>
       <c r="N21" s="50"/>
@@ -2928,10 +2930,10 @@
         <v>118</v>
       </c>
       <c r="C22" s="40"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="102"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
       <c r="F22" s="41" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G22" s="39">
         <v>2</v>
@@ -2952,10 +2954,10 @@
         <v>125</v>
       </c>
       <c r="C23" s="40"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="104"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="98"/>
       <c r="F23" s="41" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G23" s="39">
         <v>2</v>
@@ -2963,7 +2965,9 @@
       <c r="H23" s="39"/>
       <c r="I23" s="38"/>
       <c r="J23" s="39"/>
-      <c r="K23" s="40"/>
+      <c r="K23" s="40">
+        <v>1</v>
+      </c>
       <c r="L23" s="40"/>
       <c r="M23" s="40"/>
       <c r="N23" s="41"/>
@@ -2976,10 +2980,10 @@
         <v>119</v>
       </c>
       <c r="C24" s="26"/>
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="77"/>
+      <c r="E24" s="104"/>
       <c r="F24" s="27" t="s">
         <v>76</v>
       </c>
@@ -2999,7 +3003,7 @@
       <c r="N24" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="59">
+      <c r="A43" s="65">
         <v>1</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -3019,19 +3023,19 @@
       <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="60"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="71" t="s">
+      <c r="D44" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="72"/>
-      <c r="F44" s="66" t="s">
+      <c r="E44" s="69"/>
+      <c r="F44" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="68">
+      <c r="G44" s="99">
         <v>4</v>
       </c>
       <c r="H44" s="10"/>
@@ -3043,15 +3047,15 @@
       <c r="N44" s="10"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="60"/>
+      <c r="A45" s="66"/>
       <c r="B45" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="100"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
@@ -3061,15 +3065,15 @@
       <c r="N45" s="10"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="60"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="70"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="101"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
@@ -3079,7 +3083,7 @@
       <c r="N46" s="10"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="60"/>
+      <c r="A47" s="66"/>
       <c r="B47" s="10" t="s">
         <v>102</v>
       </c>
@@ -3105,19 +3109,19 @@
       <c r="N47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="60"/>
+      <c r="A48" s="66"/>
       <c r="B48" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="71" t="s">
+      <c r="D48" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="72"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="68">
+      <c r="G48" s="99">
         <v>4</v>
       </c>
       <c r="H48" s="10"/>
@@ -3129,17 +3133,17 @@
       <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="60"/>
+      <c r="A49" s="66"/>
       <c r="B49" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="74"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="73"/>
       <c r="F49" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="70"/>
+      <c r="G49" s="101"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
@@ -3149,7 +3153,7 @@
       <c r="N49" s="10"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="80"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="6" t="s">
         <v>106</v>
       </c>
@@ -3174,6 +3178,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D4:E4"/>
@@ -3186,11 +3195,6 @@
     <mergeCell ref="D8:E11"/>
     <mergeCell ref="D12:E16"/>
     <mergeCell ref="D17:E23"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:F44 F47:F50 F5:F24">
@@ -3206,7 +3210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update backlog for task sprint 3
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -1172,6 +1172,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1190,14 +1199,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1211,40 +1235,61 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1258,51 +1303,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1379,7 +1379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1414,7 +1414,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1944,18 +1944,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1983,11 +1983,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1996,9 +1996,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2016,10 +2016,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="75"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2255,7 +2255,7 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="79" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="70" t="s">
@@ -2297,7 +2297,7 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="70" t="s">
         <v>71</v>
       </c>
@@ -2411,7 +2411,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="78">
+      <c r="A14" s="72">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2431,7 +2431,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -2545,7 +2545,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -2583,7 +2583,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -2622,15 +2622,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2641,6 +2632,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2673,11 +2673,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2686,9 +2686,9 @@
       </c>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2751,10 +2751,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="75"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2842,10 +2842,10 @@
       <c r="C5" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="84"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="52" t="s">
         <v>92</v>
       </c>
@@ -2880,10 +2880,10 @@
         <v>118</v>
       </c>
       <c r="C6" s="50"/>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="86"/>
+      <c r="E6" s="88"/>
       <c r="F6" s="51" t="s">
         <v>92</v>
       </c>
@@ -2918,8 +2918,8 @@
         <v>119</v>
       </c>
       <c r="C7" s="50"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="88"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="94"/>
       <c r="F7" s="51" t="s">
         <v>92</v>
       </c>
@@ -2954,10 +2954,10 @@
         <v>108</v>
       </c>
       <c r="C8" s="50"/>
-      <c r="D8" s="85" t="s">
+      <c r="D8" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="86"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="51" t="s">
         <v>92</v>
       </c>
@@ -2980,10 +2980,10 @@
         <v>110</v>
       </c>
       <c r="C9" s="56"/>
-      <c r="D9" s="91" t="s">
+      <c r="D9" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="92"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="58" t="s">
         <v>76</v>
       </c>
@@ -3006,10 +3006,10 @@
         <v>111</v>
       </c>
       <c r="C10" s="56"/>
-      <c r="D10" s="91" t="s">
+      <c r="D10" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="92"/>
+      <c r="E10" s="86"/>
       <c r="F10" s="58" t="s">
         <v>76</v>
       </c>
@@ -3032,10 +3032,10 @@
         <v>112</v>
       </c>
       <c r="C11" s="57"/>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="92"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="58" t="s">
         <v>76</v>
       </c>
@@ -3058,8 +3058,8 @@
         <v>109</v>
       </c>
       <c r="C12" s="62"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="90"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="58"/>
       <c r="G12" s="56"/>
       <c r="H12" s="56"/>
@@ -3078,10 +3078,10 @@
         <v>113</v>
       </c>
       <c r="C13" s="56"/>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="90"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="58" t="s">
         <v>76</v>
       </c>
@@ -3116,10 +3116,10 @@
         <v>124</v>
       </c>
       <c r="C14" s="56"/>
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="90"/>
+      <c r="E14" s="82"/>
       <c r="F14" s="58" t="s">
         <v>76</v>
       </c>
@@ -3154,10 +3154,10 @@
         <v>114</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="96"/>
+      <c r="E15" s="84"/>
       <c r="F15" s="51" t="s">
         <v>92</v>
       </c>
@@ -3192,10 +3192,10 @@
         <v>115</v>
       </c>
       <c r="C16" s="57"/>
-      <c r="D16" s="89" t="s">
+      <c r="D16" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="90"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="58" t="s">
         <v>76</v>
       </c>
@@ -3230,8 +3230,8 @@
         <v>125</v>
       </c>
       <c r="C17" s="57"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="92"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
@@ -3250,10 +3250,10 @@
         <v>120</v>
       </c>
       <c r="C18" s="57"/>
-      <c r="D18" s="91" t="s">
+      <c r="D18" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="92"/>
+      <c r="E18" s="86"/>
       <c r="F18" s="58" t="s">
         <v>76</v>
       </c>
@@ -3288,10 +3288,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="66"/>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="94"/>
+      <c r="E19" s="96"/>
       <c r="F19" s="67" t="s">
         <v>66</v>
       </c>
@@ -3314,10 +3314,10 @@
         <v>122</v>
       </c>
       <c r="C20" s="50"/>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="86"/>
+      <c r="E20" s="88"/>
       <c r="F20" s="51" t="s">
         <v>92</v>
       </c>
@@ -3352,10 +3352,10 @@
         <v>116</v>
       </c>
       <c r="C21" s="57"/>
-      <c r="D21" s="91" t="s">
+      <c r="D21" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="92"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="58" t="s">
         <v>76</v>
       </c>
@@ -3390,10 +3390,10 @@
         <v>117</v>
       </c>
       <c r="C22" s="50"/>
-      <c r="D22" s="85" t="s">
+      <c r="D22" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="86"/>
+      <c r="E22" s="88"/>
       <c r="F22" s="51" t="s">
         <v>92</v>
       </c>
@@ -3428,10 +3428,10 @@
         <v>123</v>
       </c>
       <c r="C23" s="50"/>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="82"/>
+      <c r="E23" s="90"/>
       <c r="F23" s="51" t="s">
         <v>92</v>
       </c>
@@ -3698,26 +3698,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -3733,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3750,11 +3750,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -3763,9 +3763,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -3783,10 +3783,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="75"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -3822,13 +3822,13 @@
       <c r="B5" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="111"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="25" t="s">
         <v>76</v>
       </c>
@@ -3850,11 +3850,11 @@
       <c r="B6" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="110" t="s">
+      <c r="C6" s="102"/>
+      <c r="D6" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="111"/>
+      <c r="E6" s="100"/>
       <c r="F6" s="25" t="s">
         <v>76</v>
       </c>
@@ -3876,11 +3876,11 @@
       <c r="B7" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="110" t="s">
+      <c r="C7" s="102"/>
+      <c r="D7" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="111"/>
+      <c r="E7" s="100"/>
       <c r="F7" s="25" t="s">
         <v>76</v>
       </c>
@@ -3902,11 +3902,11 @@
       <c r="B8" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="113"/>
-      <c r="D8" s="114" t="s">
+      <c r="C8" s="102"/>
+      <c r="D8" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="115"/>
+      <c r="E8" s="104"/>
       <c r="F8" s="25" t="s">
         <v>76</v>
       </c>
@@ -3928,11 +3928,11 @@
       <c r="B9" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="114" t="s">
+      <c r="C9" s="102"/>
+      <c r="D9" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="115"/>
+      <c r="E9" s="104"/>
       <c r="F9" s="25" t="s">
         <v>76</v>
       </c>
@@ -3954,11 +3954,11 @@
       <c r="B10" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114" t="s">
+      <c r="C10" s="102"/>
+      <c r="D10" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="115"/>
+      <c r="E10" s="104"/>
       <c r="F10" s="25" t="s">
         <v>136</v>
       </c>
@@ -3982,13 +3982,13 @@
       <c r="B11" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="110" t="s">
+      <c r="C11" s="102"/>
+      <c r="D11" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="111"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="25" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="G11" s="21">
         <v>1</v>
@@ -4010,20 +4010,24 @@
       <c r="B12" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="110" t="s">
+      <c r="C12" s="102"/>
+      <c r="D12" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="111"/>
+      <c r="E12" s="100"/>
       <c r="F12" s="25" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="G12" s="21">
         <v>5</v>
       </c>
       <c r="H12" s="21"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="21"/>
+      <c r="I12" s="23">
+        <v>2</v>
+      </c>
+      <c r="J12" s="21">
+        <v>2</v>
+      </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
@@ -4039,19 +4043,21 @@
       <c r="C13" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="108" t="s">
+      <c r="D13" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="109"/>
+      <c r="E13" s="98"/>
       <c r="F13" s="36" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G13" s="34">
         <v>2</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
+      <c r="J13" s="34">
+        <v>2</v>
+      </c>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
@@ -4065,10 +4071,10 @@
         <v>174</v>
       </c>
       <c r="C14" s="35"/>
-      <c r="D14" s="108" t="s">
+      <c r="D14" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="109"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="36" t="s">
         <v>76</v>
       </c>
@@ -4079,7 +4085,9 @@
       <c r="I14" s="33">
         <v>2</v>
       </c>
-      <c r="J14" s="34"/>
+      <c r="J14" s="34">
+        <v>3</v>
+      </c>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
@@ -4095,10 +4103,10 @@
       <c r="C15" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D15" s="108" t="s">
+      <c r="D15" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="109"/>
+      <c r="E15" s="98"/>
       <c r="F15" s="36" t="s">
         <v>66</v>
       </c>
@@ -4123,10 +4131,10 @@
       <c r="C16" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="108" t="s">
+      <c r="D16" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="109"/>
+      <c r="E16" s="98"/>
       <c r="F16" s="36" t="s">
         <v>66</v>
       </c>
@@ -4149,10 +4157,10 @@
         <v>167</v>
       </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="109"/>
+      <c r="E17" s="98"/>
       <c r="F17" s="36" t="s">
         <v>66</v>
       </c>
@@ -4177,10 +4185,10 @@
       <c r="C18" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="108" t="s">
+      <c r="D18" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="109"/>
+      <c r="E18" s="98"/>
       <c r="F18" s="36" t="s">
         <v>66</v>
       </c>
@@ -4205,10 +4213,10 @@
       <c r="C19" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="108" t="s">
+      <c r="D19" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="109"/>
+      <c r="E19" s="98"/>
       <c r="F19" s="36" t="s">
         <v>66</v>
       </c>
@@ -4227,7 +4235,7 @@
       <c r="G20" s="32"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="78">
+      <c r="A32" s="72">
         <v>1</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -4247,15 +4255,15 @@
       <c r="N32" s="10"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="11"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="98"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="113"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
@@ -4265,15 +4273,15 @@
       <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
+      <c r="A34" s="73"/>
       <c r="B34" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C34" s="11"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="97"/>
-      <c r="G34" s="99"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="114"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
@@ -4283,15 +4291,15 @@
       <c r="N34" s="10"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="79"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C35" s="11"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="100"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="115"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
@@ -4301,7 +4309,7 @@
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
+      <c r="A36" s="73"/>
       <c r="B36" s="10" t="s">
         <v>102</v>
       </c>
@@ -4319,15 +4327,15 @@
       <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
+      <c r="A37" s="73"/>
       <c r="B37" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="102"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="107"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="98"/>
+      <c r="G37" s="113"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -4337,15 +4345,15 @@
       <c r="N37" s="10"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
+      <c r="A38" s="73"/>
       <c r="B38" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="104"/>
+      <c r="D38" s="110"/>
+      <c r="E38" s="111"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="100"/>
+      <c r="G38" s="115"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
@@ -4374,6 +4382,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E35"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:C2"/>
@@ -4388,19 +4409,6 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A32:A39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E35"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="G37:G38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32:F33 F36:F39 F5:F19">

</xml_diff>

<commit_message>
Update user Statistic, Upgrade, _UserLayout, Backlog.xlsx
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -680,7 +680,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1172,6 +1172,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1190,62 +1199,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1258,51 +1303,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1379,7 +1379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1414,7 +1414,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1630,18 +1630,18 @@
       <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.375" style="3" customWidth="1"/>
     <col min="3" max="3" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="52.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="38.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="52.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1944,18 +1944,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1970,24 +1970,24 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="6" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="37.75" style="6" customWidth="1"/>
+    <col min="3" max="3" width="45.25" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.25" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1995,10 +1995,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2016,10 +2016,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>2</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>3</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>4</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>5</v>
       </c>
@@ -2248,14 +2248,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="78" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="69" t="s">
@@ -2290,14 +2290,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="76"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="69" t="s">
         <v>71</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -2410,8 +2410,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="71">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2430,8 +2430,8 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="72"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
@@ -2468,8 +2468,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="72"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -2506,8 +2506,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="72"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -2544,8 +2544,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="72"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -2582,8 +2582,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="73"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -2622,15 +2622,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2641,6 +2632,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2660,24 +2660,24 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="6" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="37.75" style="6" customWidth="1"/>
     <col min="3" max="3" width="41" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="7" width="13.375" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2685,10 +2685,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="U3" s="28"/>
       <c r="V3" s="28"/>
       <c r="W3" s="28"/>
@@ -2741,7 +2741,7 @@
       <c r="BJ3" s="28"/>
       <c r="BK3" s="28"/>
     </row>
-    <row r="4" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2751,10 +2751,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="BJ4" s="28"/>
       <c r="BK4" s="28"/>
     </row>
-    <row r="5" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48">
         <v>1</v>
       </c>
@@ -2842,10 +2842,10 @@
       <c r="C5" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="83"/>
+      <c r="E5" s="93"/>
       <c r="F5" s="51" t="s">
         <v>92</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="N5" s="51"/>
     </row>
-    <row r="6" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48">
         <v>3</v>
       </c>
@@ -2880,10 +2880,10 @@
         <v>118</v>
       </c>
       <c r="C6" s="49"/>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="85"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="50" t="s">
         <v>92</v>
       </c>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="N6" s="51"/>
     </row>
-    <row r="7" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="48">
         <v>4</v>
       </c>
@@ -2918,8 +2918,8 @@
         <v>119</v>
       </c>
       <c r="C7" s="49"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="50" t="s">
         <v>92</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="N7" s="51"/>
     </row>
-    <row r="8" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="48">
         <v>5</v>
       </c>
@@ -2954,10 +2954,10 @@
         <v>108</v>
       </c>
       <c r="C8" s="49"/>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="85"/>
+      <c r="E8" s="87"/>
       <c r="F8" s="50" t="s">
         <v>92</v>
       </c>
@@ -2972,7 +2972,7 @@
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
     </row>
-    <row r="9" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="54">
         <v>6</v>
       </c>
@@ -2980,10 +2980,10 @@
         <v>110</v>
       </c>
       <c r="C9" s="55"/>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="89"/>
+      <c r="E9" s="85"/>
       <c r="F9" s="57" t="s">
         <v>76</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="M9" s="55"/>
       <c r="N9" s="55"/>
     </row>
-    <row r="10" spans="1:63" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="54">
         <v>7</v>
       </c>
@@ -3006,10 +3006,10 @@
         <v>111</v>
       </c>
       <c r="C10" s="55"/>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="89"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="57" t="s">
         <v>76</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="M10" s="55"/>
       <c r="N10" s="55"/>
     </row>
-    <row r="11" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="54">
         <v>8</v>
       </c>
@@ -3032,10 +3032,10 @@
         <v>112</v>
       </c>
       <c r="C11" s="56"/>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="89"/>
+      <c r="E11" s="85"/>
       <c r="F11" s="57" t="s">
         <v>76</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="M11" s="55"/>
       <c r="N11" s="55"/>
     </row>
-    <row r="12" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54">
         <v>9</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="M12" s="55"/>
       <c r="N12" s="55"/>
     </row>
-    <row r="13" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54">
         <v>10</v>
       </c>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="N13" s="55"/>
     </row>
-    <row r="14" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="54">
         <v>11</v>
       </c>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="N14" s="55"/>
     </row>
-    <row r="15" spans="1:63" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="48">
         <v>12</v>
       </c>
@@ -3154,10 +3154,10 @@
         <v>114</v>
       </c>
       <c r="C15" s="49"/>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="91"/>
+      <c r="E15" s="83"/>
       <c r="F15" s="50" t="s">
         <v>92</v>
       </c>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="N15" s="50"/>
     </row>
-    <row r="16" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="54">
         <v>13</v>
       </c>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="N16" s="57"/>
     </row>
-    <row r="17" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54">
         <v>14</v>
       </c>
@@ -3230,8 +3230,8 @@
         <v>125</v>
       </c>
       <c r="C17" s="56"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
       <c r="F17" s="57"/>
       <c r="G17" s="55"/>
       <c r="H17" s="55"/>
@@ -3242,7 +3242,7 @@
       <c r="M17" s="56"/>
       <c r="N17" s="57"/>
     </row>
-    <row r="18" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="54">
         <v>15</v>
       </c>
@@ -3250,10 +3250,10 @@
         <v>120</v>
       </c>
       <c r="C18" s="56"/>
-      <c r="D18" s="88" t="s">
+      <c r="D18" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="89"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="57" t="s">
         <v>76</v>
       </c>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="N18" s="57"/>
     </row>
-    <row r="19" spans="1:63" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" s="67" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="63">
         <v>16</v>
       </c>
@@ -3288,10 +3288,10 @@
         <v>121</v>
       </c>
       <c r="C19" s="65"/>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="90" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="95"/>
+      <c r="E19" s="91"/>
       <c r="F19" s="66" t="s">
         <v>66</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="M19" s="65"/>
       <c r="N19" s="66"/>
     </row>
-    <row r="20" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48">
         <v>17</v>
       </c>
@@ -3314,10 +3314,10 @@
         <v>122</v>
       </c>
       <c r="C20" s="49"/>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="85"/>
+      <c r="E20" s="87"/>
       <c r="F20" s="50" t="s">
         <v>92</v>
       </c>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="N20" s="50"/>
     </row>
-    <row r="21" spans="1:63" s="53" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" s="53" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54">
         <v>18</v>
       </c>
@@ -3352,10 +3352,10 @@
         <v>116</v>
       </c>
       <c r="C21" s="56"/>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="89"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="57" t="s">
         <v>76</v>
       </c>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="N21" s="57"/>
     </row>
-    <row r="22" spans="1:63" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="48">
         <v>19</v>
       </c>
@@ -3390,10 +3390,10 @@
         <v>117</v>
       </c>
       <c r="C22" s="49"/>
-      <c r="D22" s="84" t="s">
+      <c r="D22" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="85"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="50" t="s">
         <v>92</v>
       </c>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="N22" s="50"/>
     </row>
-    <row r="23" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48">
         <v>20</v>
       </c>
@@ -3428,10 +3428,10 @@
         <v>123</v>
       </c>
       <c r="C23" s="49"/>
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="93"/>
+      <c r="E23" s="89"/>
       <c r="F23" s="50" t="s">
         <v>92</v>
       </c>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="N23" s="50"/>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.2">
       <c r="O24" s="28"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
@@ -3509,7 +3509,7 @@
       <c r="BJ24" s="28"/>
       <c r="BK24" s="28"/>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B25" s="38" t="s">
         <v>163</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>71</v>
       </c>
@@ -3698,6 +3698,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D21:E21"/>
@@ -3708,16 +3718,6 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -3733,28 +3733,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="6" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="37.75" style="6" customWidth="1"/>
     <col min="3" max="3" width="41" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="7" width="13.375" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -3762,10 +3762,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>42065</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3783,10 +3783,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -3815,20 +3815,20 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>1</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D5" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="110"/>
+      <c r="E5" s="99"/>
       <c r="F5" s="25" t="s">
         <v>76</v>
       </c>
@@ -3843,18 +3843,18 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
     </row>
-    <row r="6" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="109" t="s">
+      <c r="C6" s="101"/>
+      <c r="D6" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="110"/>
+      <c r="E6" s="99"/>
       <c r="F6" s="25" t="s">
         <v>76</v>
       </c>
@@ -3869,18 +3869,18 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
     </row>
-    <row r="7" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>3</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="109" t="s">
+      <c r="C7" s="101"/>
+      <c r="D7" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="110"/>
+      <c r="E7" s="99"/>
       <c r="F7" s="25" t="s">
         <v>76</v>
       </c>
@@ -3895,20 +3895,20 @@
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>4</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="113" t="s">
+      <c r="C8" s="101"/>
+      <c r="D8" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="114"/>
+      <c r="E8" s="103"/>
       <c r="F8" s="25" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="G8" s="21">
         <v>1</v>
@@ -3916,25 +3916,27 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="21">
+        <v>1</v>
+      </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
     </row>
-    <row r="9" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>5</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="113" t="s">
+      <c r="C9" s="101"/>
+      <c r="D9" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="114"/>
+      <c r="E9" s="103"/>
       <c r="F9" s="25" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="G9" s="21">
         <v>1</v>
@@ -3942,23 +3944,25 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="21">
+        <v>1</v>
+      </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>6</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="113" t="s">
+      <c r="C10" s="101"/>
+      <c r="D10" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="114"/>
+      <c r="E10" s="103"/>
       <c r="F10" s="25" t="s">
         <v>136</v>
       </c>
@@ -3975,18 +3979,18 @@
       <c r="M10" s="27"/>
       <c r="N10" s="25"/>
     </row>
-    <row r="11" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>7</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="112"/>
-      <c r="D11" s="109" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="110"/>
+      <c r="E11" s="99"/>
       <c r="F11" s="25" t="s">
         <v>92</v>
       </c>
@@ -4003,18 +4007,18 @@
       <c r="M11" s="27"/>
       <c r="N11" s="25"/>
     </row>
-    <row r="12" spans="1:14" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>8</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="109" t="s">
+      <c r="C12" s="101"/>
+      <c r="D12" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="110"/>
+      <c r="E12" s="99"/>
       <c r="F12" s="25" t="s">
         <v>136</v>
       </c>
@@ -4033,7 +4037,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="25"/>
     </row>
-    <row r="13" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32">
         <v>9</v>
       </c>
@@ -4043,10 +4047,10 @@
       <c r="C13" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="108"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="35" t="s">
         <v>76</v>
       </c>
@@ -4063,7 +4067,7 @@
       <c r="M13" s="34"/>
       <c r="N13" s="35"/>
     </row>
-    <row r="14" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32">
         <v>10</v>
       </c>
@@ -4071,10 +4075,10 @@
         <v>174</v>
       </c>
       <c r="C14" s="34"/>
-      <c r="D14" s="107" t="s">
+      <c r="D14" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="108"/>
+      <c r="E14" s="97"/>
       <c r="F14" s="35" t="s">
         <v>76</v>
       </c>
@@ -4093,7 +4097,7 @@
       <c r="M14" s="34"/>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:14" s="36" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="36" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A15" s="32">
         <v>11</v>
       </c>
@@ -4103,10 +4107,10 @@
       <c r="C15" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="D15" s="107" t="s">
+      <c r="D15" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="108"/>
+      <c r="E15" s="97"/>
       <c r="F15" s="35" t="s">
         <v>66</v>
       </c>
@@ -4121,7 +4125,7 @@
       <c r="M15" s="34"/>
       <c r="N15" s="35"/>
     </row>
-    <row r="16" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32">
         <v>12</v>
       </c>
@@ -4131,10 +4135,10 @@
       <c r="C16" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="107" t="s">
+      <c r="D16" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="108"/>
+      <c r="E16" s="97"/>
       <c r="F16" s="35" t="s">
         <v>76</v>
       </c>
@@ -4149,7 +4153,7 @@
       <c r="M16" s="34"/>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32">
         <v>13</v>
       </c>
@@ -4157,10 +4161,10 @@
         <v>167</v>
       </c>
       <c r="C17" s="34"/>
-      <c r="D17" s="107" t="s">
+      <c r="D17" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="108"/>
+      <c r="E17" s="97"/>
       <c r="F17" s="35" t="s">
         <v>66</v>
       </c>
@@ -4175,7 +4179,7 @@
       <c r="M17" s="34"/>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="32">
         <v>14</v>
       </c>
@@ -4185,10 +4189,10 @@
       <c r="C18" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="107" t="s">
+      <c r="D18" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="108"/>
+      <c r="E18" s="97"/>
       <c r="F18" s="35" t="s">
         <v>66</v>
       </c>
@@ -4203,7 +4207,7 @@
       <c r="M18" s="34"/>
       <c r="N18" s="35"/>
     </row>
-    <row r="19" spans="1:14" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32">
         <v>15</v>
       </c>
@@ -4213,10 +4217,10 @@
       <c r="C19" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="107" t="s">
+      <c r="D19" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="108"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="35" t="s">
         <v>66</v>
       </c>
@@ -4231,7 +4235,7 @@
       <c r="M19" s="34"/>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32">
         <v>16</v>
       </c>
@@ -4239,10 +4243,10 @@
         <v>180</v>
       </c>
       <c r="C20" s="34"/>
-      <c r="D20" s="107" t="s">
+      <c r="D20" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="108"/>
+      <c r="E20" s="97"/>
       <c r="F20" s="35" t="s">
         <v>66</v>
       </c>
@@ -4257,8 +4261,8 @@
       <c r="M20" s="34"/>
       <c r="N20" s="35"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="77">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="71">
         <v>1</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -4277,16 +4281,16 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="78"/>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="72"/>
       <c r="B33" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="11"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="97"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="112"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
@@ -4295,16 +4299,16 @@
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="72"/>
       <c r="B34" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C34" s="11"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="98"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="113"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
@@ -4313,16 +4317,16 @@
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="72"/>
       <c r="B35" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C35" s="11"/>
-      <c r="D35" s="102"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="99"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="114"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
@@ -4331,8 +4335,8 @@
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="78"/>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="72"/>
       <c r="B36" s="10" t="s">
         <v>102</v>
       </c>
@@ -4349,16 +4353,16 @@
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="72"/>
       <c r="B37" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="101"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="106"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="97"/>
+      <c r="G37" s="112"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -4367,16 +4371,16 @@
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="72"/>
       <c r="B38" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="102"/>
-      <c r="E38" s="103"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="110"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="99"/>
+      <c r="G38" s="114"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
@@ -4385,7 +4389,7 @@
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="104"/>
       <c r="B39" s="6" t="s">
         <v>105</v>
@@ -4405,6 +4409,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E35"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:C2"/>
@@ -4419,20 +4437,6 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A32:A39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E35"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="G37:G38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32:F33 F36:F39 F5:F20">
@@ -4452,20 +4456,20 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="14.25" style="18" customWidth="1"/>
     <col min="2" max="2" width="20" style="18" customWidth="1"/>
     <col min="3" max="3" width="48" style="18" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="18" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="18"/>
+    <col min="4" max="4" width="56.625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="18" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="18"/>
     <col min="8" max="8" width="56" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="18" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.85546875" style="18" customWidth="1"/>
-    <col min="12" max="12" width="51.140625" style="18" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="18"/>
+    <col min="10" max="10" width="20.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="51.125" style="18" customWidth="1"/>
+    <col min="13" max="16384" width="9.125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
@@ -4738,7 +4742,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.2">
       <c r="H21" s="29" t="s">
         <v>111</v>
       </c>
@@ -4752,7 +4756,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" ht="45" x14ac:dyDescent="0.2">
       <c r="H22" s="29" t="s">
         <v>112</v>
       </c>
@@ -4766,7 +4770,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.2">
       <c r="H23" s="29" t="s">
         <v>113</v>
       </c>
@@ -4914,27 +4918,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Update task Report 3
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>Sprint 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review </t>
   </si>
   <si>
     <t>Not complete in sprint 1</t>
@@ -841,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -891,16 +888,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1025,6 +1016,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1034,6 +1031,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1043,48 +1058,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1097,17 +1106,26 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1139,41 +1157,53 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1800,18 +1830,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1839,11 +1869,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1852,9 +1882,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1872,10 +1902,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2033,7 +2063,7 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="10" t="s">
@@ -2073,7 +2103,7 @@
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="10" t="s">
@@ -2111,7 +2141,7 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="70" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="64" t="s">
@@ -2153,7 +2183,7 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="64" t="s">
         <v>71</v>
       </c>
@@ -2195,7 +2225,7 @@
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="65"/>
       <c r="F12" s="10" t="s">
@@ -2267,7 +2297,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="66">
+      <c r="A14" s="72">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2287,13 +2317,13 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="10" t="s">
@@ -2325,7 +2355,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -2363,7 +2393,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="67"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -2401,7 +2431,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -2439,7 +2469,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -2478,6 +2508,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -2488,15 +2527,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -2529,11 +2559,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -2542,9 +2572,9 @@
       </c>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -2553,49 +2583,49 @@
       </c>
     </row>
     <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="26"/>
-      <c r="AQ3" s="26"/>
-      <c r="AR3" s="26"/>
-      <c r="AS3" s="26"/>
-      <c r="AT3" s="26"/>
-      <c r="AU3" s="26"/>
-      <c r="AV3" s="26"/>
-      <c r="AW3" s="26"/>
-      <c r="AX3" s="26"/>
-      <c r="AY3" s="26"/>
-      <c r="AZ3" s="26"/>
-      <c r="BA3" s="26"/>
-      <c r="BB3" s="26"/>
-      <c r="BC3" s="26"/>
-      <c r="BD3" s="26"/>
-      <c r="BE3" s="26"/>
-      <c r="BF3" s="26"/>
-      <c r="BG3" s="26"/>
-      <c r="BH3" s="26"/>
-      <c r="BI3" s="26"/>
-      <c r="BJ3" s="26"/>
-      <c r="BK3" s="26"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24"/>
+      <c r="AX3" s="24"/>
+      <c r="AY3" s="24"/>
+      <c r="AZ3" s="24"/>
+      <c r="BA3" s="24"/>
+      <c r="BB3" s="24"/>
+      <c r="BC3" s="24"/>
+      <c r="BD3" s="24"/>
+      <c r="BE3" s="24"/>
+      <c r="BF3" s="24"/>
+      <c r="BG3" s="24"/>
+      <c r="BH3" s="24"/>
+      <c r="BI3" s="24"/>
+      <c r="BJ3" s="24"/>
+      <c r="BK3" s="24"/>
     </row>
     <row r="4" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -2607,10 +2637,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -2638,909 +2668,909 @@
       <c r="N4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="26"/>
-      <c r="AM4" s="26"/>
-      <c r="AN4" s="26"/>
-      <c r="AO4" s="26"/>
-      <c r="AP4" s="26"/>
-      <c r="AQ4" s="26"/>
-      <c r="AR4" s="26"/>
-      <c r="AS4" s="26"/>
-      <c r="AT4" s="26"/>
-      <c r="AU4" s="26"/>
-      <c r="AV4" s="26"/>
-      <c r="AW4" s="26"/>
-      <c r="AX4" s="26"/>
-      <c r="AY4" s="26"/>
-      <c r="AZ4" s="26"/>
-      <c r="BA4" s="26"/>
-      <c r="BB4" s="26"/>
-      <c r="BC4" s="26"/>
-      <c r="BD4" s="26"/>
-      <c r="BE4" s="26"/>
-      <c r="BF4" s="26"/>
-      <c r="BG4" s="26"/>
-      <c r="BH4" s="26"/>
-      <c r="BI4" s="26"/>
-      <c r="BJ4" s="26"/>
-      <c r="BK4" s="26"/>
-    </row>
-    <row r="5" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
+      <c r="AW4" s="24"/>
+      <c r="AX4" s="24"/>
+      <c r="AY4" s="24"/>
+      <c r="AZ4" s="24"/>
+      <c r="BA4" s="24"/>
+      <c r="BB4" s="24"/>
+      <c r="BC4" s="24"/>
+      <c r="BD4" s="24"/>
+      <c r="BE4" s="24"/>
+      <c r="BF4" s="24"/>
+      <c r="BG4" s="24"/>
+      <c r="BH4" s="24"/>
+      <c r="BI4" s="24"/>
+      <c r="BJ4" s="24"/>
+      <c r="BK4" s="24"/>
+    </row>
+    <row r="5" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
         <v>1</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="E5" s="78"/>
+      <c r="F5" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="49">
+        <v>2</v>
+      </c>
+      <c r="H5" s="38">
+        <v>2</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0</v>
+      </c>
+      <c r="J5" s="38">
+        <v>0</v>
+      </c>
+      <c r="K5" s="38">
+        <v>0</v>
+      </c>
+      <c r="L5" s="38">
+        <v>0</v>
+      </c>
+      <c r="M5" s="38">
+        <v>0</v>
+      </c>
+      <c r="N5" s="38"/>
+    </row>
+    <row r="6" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="80"/>
+      <c r="F6" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="38">
+        <v>2</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0</v>
+      </c>
+      <c r="I6" s="38">
+        <v>2</v>
+      </c>
+      <c r="J6" s="38">
+        <v>0</v>
+      </c>
+      <c r="K6" s="38">
+        <v>0</v>
+      </c>
+      <c r="L6" s="38">
+        <v>0</v>
+      </c>
+      <c r="M6" s="38">
+        <v>0</v>
+      </c>
+      <c r="N6" s="38"/>
+    </row>
+    <row r="7" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="38">
+        <v>2</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0</v>
+      </c>
+      <c r="J7" s="38">
+        <v>2</v>
+      </c>
+      <c r="K7" s="38">
+        <v>0</v>
+      </c>
+      <c r="L7" s="38">
+        <v>0</v>
+      </c>
+      <c r="M7" s="38">
+        <v>0</v>
+      </c>
+      <c r="N7" s="38"/>
+    </row>
+    <row r="8" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="88"/>
-      <c r="F5" s="40" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="80"/>
+      <c r="F8" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="51">
-        <v>2</v>
-      </c>
-      <c r="H5" s="40">
-        <v>2</v>
-      </c>
-      <c r="I5" s="40">
-        <v>0</v>
-      </c>
-      <c r="J5" s="40">
-        <v>0</v>
-      </c>
-      <c r="K5" s="40">
-        <v>0</v>
-      </c>
-      <c r="L5" s="40">
-        <v>0</v>
-      </c>
-      <c r="M5" s="40">
-        <v>0</v>
-      </c>
-      <c r="N5" s="40"/>
-    </row>
-    <row r="6" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
-        <v>3</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="40">
-        <v>2</v>
-      </c>
-      <c r="H6" s="40">
-        <v>0</v>
-      </c>
-      <c r="I6" s="40">
-        <v>2</v>
-      </c>
-      <c r="J6" s="40">
-        <v>0</v>
-      </c>
-      <c r="K6" s="40">
-        <v>0</v>
-      </c>
-      <c r="L6" s="40">
-        <v>0</v>
-      </c>
-      <c r="M6" s="40">
-        <v>0</v>
-      </c>
-      <c r="N6" s="40"/>
-    </row>
-    <row r="7" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
-        <v>4</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="40">
-        <v>2</v>
-      </c>
-      <c r="H7" s="40">
-        <v>0</v>
-      </c>
-      <c r="I7" s="40">
-        <v>0</v>
-      </c>
-      <c r="J7" s="40">
-        <v>2</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40"/>
-    </row>
-    <row r="8" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
-        <v>5</v>
-      </c>
-      <c r="B8" s="40" t="s">
+      <c r="G8" s="38">
+        <v>2</v>
+      </c>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+    </row>
+    <row r="9" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="41">
+        <v>6</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="D9" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="84"/>
+      <c r="F9" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="42">
+        <v>2</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+    </row>
+    <row r="10" spans="1:63" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="41">
+        <v>7</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="84"/>
+      <c r="F10" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="42">
+        <v>2</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+    </row>
+    <row r="11" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41">
+        <v>8</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="84"/>
+      <c r="F11" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="42">
+        <v>2</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+    </row>
+    <row r="12" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
+        <v>9</v>
+      </c>
+      <c r="B12" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="82"/>
-      <c r="F8" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="40">
-        <v>2</v>
-      </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-    </row>
-    <row r="9" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
-        <v>6</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="44">
-        <v>2</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-    </row>
-    <row r="10" spans="1:63" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
-        <v>7</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="44">
-        <v>2</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-    </row>
-    <row r="11" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
-        <v>8</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="44">
-        <v>2</v>
-      </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-    </row>
-    <row r="12" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
-        <v>9</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="50"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="75"/>
       <c r="E12" s="76"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-    </row>
-    <row r="13" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43">
+      <c r="F12" s="44"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+    </row>
+    <row r="13" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41">
         <v>10</v>
       </c>
-      <c r="B13" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="44"/>
+      <c r="B13" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="42"/>
       <c r="D13" s="75" t="s">
         <v>69</v>
       </c>
       <c r="E13" s="76"/>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="44">
-        <v>2</v>
-      </c>
-      <c r="H13" s="44">
-        <v>0</v>
-      </c>
-      <c r="I13" s="44">
-        <v>0</v>
-      </c>
-      <c r="J13" s="44">
-        <v>0</v>
-      </c>
-      <c r="K13" s="44">
-        <v>0</v>
-      </c>
-      <c r="L13" s="44">
-        <v>2</v>
-      </c>
-      <c r="M13" s="44">
-        <v>0</v>
-      </c>
-      <c r="N13" s="44"/>
-    </row>
-    <row r="14" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="G13" s="42">
+        <v>2</v>
+      </c>
+      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="I13" s="42">
+        <v>0</v>
+      </c>
+      <c r="J13" s="42">
+        <v>0</v>
+      </c>
+      <c r="K13" s="42">
+        <v>0</v>
+      </c>
+      <c r="L13" s="42">
+        <v>2</v>
+      </c>
+      <c r="M13" s="42">
+        <v>0</v>
+      </c>
+      <c r="N13" s="42"/>
+    </row>
+    <row r="14" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41">
         <v>11</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="44"/>
+      <c r="B14" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="42"/>
       <c r="D14" s="75" t="s">
         <v>69</v>
       </c>
       <c r="E14" s="76"/>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="44">
-        <v>2</v>
-      </c>
-      <c r="H14" s="44">
-        <v>0</v>
-      </c>
-      <c r="I14" s="44">
-        <v>0</v>
-      </c>
-      <c r="J14" s="44">
-        <v>0</v>
-      </c>
-      <c r="K14" s="44">
-        <v>0</v>
-      </c>
-      <c r="L14" s="44">
+      <c r="G14" s="42">
+        <v>2</v>
+      </c>
+      <c r="H14" s="42">
+        <v>0</v>
+      </c>
+      <c r="I14" s="42">
+        <v>0</v>
+      </c>
+      <c r="J14" s="42">
+        <v>0</v>
+      </c>
+      <c r="K14" s="42">
+        <v>0</v>
+      </c>
+      <c r="L14" s="42">
         <v>1</v>
       </c>
-      <c r="M14" s="44">
+      <c r="M14" s="42">
         <v>1</v>
       </c>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15" spans="1:63" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="N14" s="42"/>
+    </row>
+    <row r="15" spans="1:63" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
         <v>12</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="86"/>
+      <c r="F15" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="38">
+        <v>2</v>
+      </c>
+      <c r="H15" s="38">
+        <v>0</v>
+      </c>
+      <c r="I15" s="38">
+        <v>0</v>
+      </c>
+      <c r="J15" s="38">
+        <v>0</v>
+      </c>
+      <c r="K15" s="38">
+        <v>0</v>
+      </c>
+      <c r="L15" s="38">
+        <v>0</v>
+      </c>
+      <c r="M15" s="36">
+        <v>2</v>
+      </c>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41">
+        <v>13</v>
+      </c>
+      <c r="B16" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="40">
-        <v>2</v>
-      </c>
-      <c r="H15" s="40">
-        <v>0</v>
-      </c>
-      <c r="I15" s="40">
-        <v>0</v>
-      </c>
-      <c r="J15" s="40">
-        <v>0</v>
-      </c>
-      <c r="K15" s="40">
-        <v>0</v>
-      </c>
-      <c r="L15" s="40">
-        <v>0</v>
-      </c>
-      <c r="M15" s="38">
-        <v>2</v>
-      </c>
-      <c r="N15" s="39"/>
-    </row>
-    <row r="16" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
-        <v>13</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="75" t="s">
         <v>69</v>
       </c>
       <c r="E16" s="76"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="44">
-        <v>2</v>
-      </c>
-      <c r="H16" s="44">
-        <v>0</v>
-      </c>
-      <c r="I16" s="43">
-        <v>0</v>
-      </c>
-      <c r="J16" s="44">
-        <v>0</v>
-      </c>
-      <c r="K16" s="45">
-        <v>0</v>
-      </c>
-      <c r="L16" s="45">
-        <v>0</v>
-      </c>
-      <c r="M16" s="45">
+      <c r="G16" s="42">
+        <v>2</v>
+      </c>
+      <c r="H16" s="42">
+        <v>0</v>
+      </c>
+      <c r="I16" s="41">
+        <v>0</v>
+      </c>
+      <c r="J16" s="42">
+        <v>0</v>
+      </c>
+      <c r="K16" s="43">
+        <v>0</v>
+      </c>
+      <c r="L16" s="43">
+        <v>0</v>
+      </c>
+      <c r="M16" s="43">
         <v>1</v>
       </c>
-      <c r="N16" s="46"/>
-    </row>
-    <row r="17" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+      <c r="N16" s="44"/>
+    </row>
+    <row r="17" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41">
         <v>14</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="44"/>
+    </row>
+    <row r="18" spans="1:63" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41">
+        <v>15</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="84"/>
+      <c r="F18" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="42">
+        <v>2</v>
+      </c>
+      <c r="H18" s="42">
+        <v>0</v>
+      </c>
+      <c r="I18" s="41">
+        <v>0</v>
+      </c>
+      <c r="J18" s="42">
+        <v>1</v>
+      </c>
+      <c r="K18" s="43">
+        <v>0</v>
+      </c>
+      <c r="L18" s="43">
+        <v>0</v>
+      </c>
+      <c r="M18" s="43">
+        <v>1</v>
+      </c>
+      <c r="N18" s="44"/>
+    </row>
+    <row r="19" spans="1:63" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="50">
+        <v>16</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="52"/>
+      <c r="D19" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="90"/>
+      <c r="F19" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="51">
+        <v>2</v>
+      </c>
+      <c r="H19" s="51"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="53"/>
+    </row>
+    <row r="20" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35">
+        <v>17</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="80"/>
+      <c r="F20" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="38">
+        <v>2</v>
+      </c>
+      <c r="H20" s="38">
+        <v>0</v>
+      </c>
+      <c r="I20" s="35">
+        <v>0</v>
+      </c>
+      <c r="J20" s="38">
+        <v>2</v>
+      </c>
+      <c r="K20" s="36">
+        <v>2</v>
+      </c>
+      <c r="L20" s="36">
+        <v>1</v>
+      </c>
+      <c r="M20" s="36">
+        <v>0</v>
+      </c>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="1:63" s="40" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41">
+        <v>18</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="84"/>
+      <c r="F21" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="42">
+        <v>2</v>
+      </c>
+      <c r="H21" s="42">
+        <v>0</v>
+      </c>
+      <c r="I21" s="41">
+        <v>0</v>
+      </c>
+      <c r="J21" s="42">
+        <v>0</v>
+      </c>
+      <c r="K21" s="43">
+        <v>0</v>
+      </c>
+      <c r="L21" s="43">
+        <v>0</v>
+      </c>
+      <c r="M21" s="43">
+        <v>1</v>
+      </c>
+      <c r="N21" s="44"/>
+    </row>
+    <row r="22" spans="1:63" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="35">
+        <v>19</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="80"/>
+      <c r="F22" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="38">
+        <v>2</v>
+      </c>
+      <c r="H22" s="38">
+        <v>0</v>
+      </c>
+      <c r="I22" s="35">
+        <v>0</v>
+      </c>
+      <c r="J22" s="38">
+        <v>0</v>
+      </c>
+      <c r="K22" s="36">
+        <v>2</v>
+      </c>
+      <c r="L22" s="36">
+        <v>2</v>
+      </c>
+      <c r="M22" s="36">
+        <v>0</v>
+      </c>
+      <c r="N22" s="37"/>
+    </row>
+    <row r="23" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
+        <v>20</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="88"/>
+      <c r="F23" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="38">
+        <v>2</v>
+      </c>
+      <c r="H23" s="38">
+        <v>0</v>
+      </c>
+      <c r="I23" s="35">
+        <v>0</v>
+      </c>
+      <c r="J23" s="38">
+        <v>0</v>
+      </c>
+      <c r="K23" s="36">
+        <v>0</v>
+      </c>
+      <c r="L23" s="36">
+        <v>1</v>
+      </c>
+      <c r="M23" s="36">
+        <v>2</v>
+      </c>
+      <c r="N23" s="37"/>
+    </row>
+    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="24"/>
+      <c r="AG24" s="24"/>
+      <c r="AH24" s="24"/>
+      <c r="AI24" s="24"/>
+      <c r="AJ24" s="24"/>
+      <c r="AK24" s="24"/>
+      <c r="AL24" s="24"/>
+      <c r="AM24" s="24"/>
+      <c r="AN24" s="24"/>
+      <c r="AO24" s="24"/>
+      <c r="AP24" s="24"/>
+      <c r="AQ24" s="24"/>
+      <c r="AR24" s="24"/>
+      <c r="AS24" s="24"/>
+      <c r="AT24" s="24"/>
+      <c r="AU24" s="24"/>
+      <c r="AV24" s="24"/>
+      <c r="AW24" s="24"/>
+      <c r="AX24" s="24"/>
+      <c r="AY24" s="24"/>
+      <c r="AZ24" s="24"/>
+      <c r="BA24" s="24"/>
+      <c r="BB24" s="24"/>
+      <c r="BC24" s="24"/>
+      <c r="BD24" s="24"/>
+      <c r="BE24" s="24"/>
+      <c r="BF24" s="24"/>
+      <c r="BG24" s="24"/>
+      <c r="BH24" s="24"/>
+      <c r="BI24" s="24"/>
+      <c r="BJ24" s="24"/>
+      <c r="BK24" s="24"/>
+    </row>
+    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="46"/>
-    </row>
-    <row r="18" spans="1:63" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
-        <v>15</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="79" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="80"/>
-      <c r="F18" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="44">
-        <v>2</v>
-      </c>
-      <c r="H18" s="44">
-        <v>0</v>
-      </c>
-      <c r="I18" s="43">
-        <v>0</v>
-      </c>
-      <c r="J18" s="44">
-        <v>1</v>
-      </c>
-      <c r="K18" s="45">
-        <v>0</v>
-      </c>
-      <c r="L18" s="45">
-        <v>0</v>
-      </c>
-      <c r="M18" s="45">
-        <v>1</v>
-      </c>
-      <c r="N18" s="46"/>
-    </row>
-    <row r="19" spans="1:63" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
-        <v>16</v>
-      </c>
-      <c r="B19" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="53">
-        <v>2</v>
-      </c>
-      <c r="H19" s="53"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="55"/>
-    </row>
-    <row r="20" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37">
-        <v>17</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="40">
-        <v>2</v>
-      </c>
-      <c r="H20" s="40">
-        <v>0</v>
-      </c>
-      <c r="I20" s="37">
-        <v>0</v>
-      </c>
-      <c r="J20" s="40">
-        <v>2</v>
-      </c>
-      <c r="K20" s="38">
-        <v>2</v>
-      </c>
-      <c r="L20" s="38">
-        <v>1</v>
-      </c>
-      <c r="M20" s="38">
-        <v>0</v>
-      </c>
-      <c r="N20" s="39"/>
-    </row>
-    <row r="21" spans="1:63" s="42" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
-        <v>18</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="79" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="80"/>
-      <c r="F21" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="44">
-        <v>2</v>
-      </c>
-      <c r="H21" s="44">
-        <v>0</v>
-      </c>
-      <c r="I21" s="43">
-        <v>0</v>
-      </c>
-      <c r="J21" s="44">
-        <v>0</v>
-      </c>
-      <c r="K21" s="45">
-        <v>0</v>
-      </c>
-      <c r="L21" s="45">
-        <v>0</v>
-      </c>
-      <c r="M21" s="45">
-        <v>1</v>
-      </c>
-      <c r="N21" s="46"/>
-    </row>
-    <row r="22" spans="1:63" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="37">
-        <v>19</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="82"/>
-      <c r="F22" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="40">
-        <v>2</v>
-      </c>
-      <c r="H22" s="40">
-        <v>0</v>
-      </c>
-      <c r="I22" s="37">
-        <v>0</v>
-      </c>
-      <c r="J22" s="40">
-        <v>0</v>
-      </c>
-      <c r="K22" s="38">
-        <v>2</v>
-      </c>
-      <c r="L22" s="38">
-        <v>2</v>
-      </c>
-      <c r="M22" s="38">
-        <v>0</v>
-      </c>
-      <c r="N22" s="39"/>
-    </row>
-    <row r="23" spans="1:63" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37">
-        <v>20</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="83" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="40">
-        <v>2</v>
-      </c>
-      <c r="H23" s="40">
-        <v>0</v>
-      </c>
-      <c r="I23" s="37">
-        <v>0</v>
-      </c>
-      <c r="J23" s="40">
-        <v>0</v>
-      </c>
-      <c r="K23" s="38">
-        <v>0</v>
-      </c>
-      <c r="L23" s="38">
-        <v>1</v>
-      </c>
-      <c r="M23" s="38">
-        <v>2</v>
-      </c>
-      <c r="N23" s="39"/>
-    </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
-      <c r="AH24" s="26"/>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="26"/>
-      <c r="AM24" s="26"/>
-      <c r="AN24" s="26"/>
-      <c r="AO24" s="26"/>
-      <c r="AP24" s="26"/>
-      <c r="AQ24" s="26"/>
-      <c r="AR24" s="26"/>
-      <c r="AS24" s="26"/>
-      <c r="AT24" s="26"/>
-      <c r="AU24" s="26"/>
-      <c r="AV24" s="26"/>
-      <c r="AW24" s="26"/>
-      <c r="AX24" s="26"/>
-      <c r="AY24" s="26"/>
-      <c r="AZ24" s="26"/>
-      <c r="BA24" s="26"/>
-      <c r="BB24" s="26"/>
-      <c r="BC24" s="26"/>
-      <c r="BD24" s="26"/>
-      <c r="BE24" s="26"/>
-      <c r="BF24" s="26"/>
-      <c r="BG24" s="26"/>
-      <c r="BH24" s="26"/>
-      <c r="BI24" s="26"/>
-      <c r="BJ24" s="26"/>
-      <c r="BK24" s="26"/>
-    </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26"/>
-      <c r="AD25" s="26"/>
-      <c r="AE25" s="26"/>
-      <c r="AF25" s="26"/>
-      <c r="AG25" s="26"/>
-      <c r="AH25" s="26"/>
-      <c r="AI25" s="26"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="26"/>
-      <c r="AM25" s="26"/>
-      <c r="AN25" s="26"/>
-      <c r="AO25" s="26"/>
-      <c r="AP25" s="26"/>
-      <c r="AQ25" s="26"/>
-      <c r="AR25" s="26"/>
-      <c r="AS25" s="26"/>
-      <c r="AT25" s="26"/>
-      <c r="AU25" s="26"/>
-      <c r="AV25" s="26"/>
-      <c r="AW25" s="26"/>
-      <c r="AX25" s="26"/>
-      <c r="AY25" s="26"/>
-      <c r="AZ25" s="26"/>
-      <c r="BA25" s="26"/>
-      <c r="BB25" s="26"/>
-      <c r="BC25" s="26"/>
-      <c r="BD25" s="26"/>
-      <c r="BE25" s="26"/>
-      <c r="BF25" s="26"/>
-      <c r="BG25" s="26"/>
-      <c r="BH25" s="26"/>
-      <c r="BI25" s="26"/>
-      <c r="BJ25" s="26"/>
-      <c r="BK25" s="26"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="24"/>
+      <c r="AG25" s="24"/>
+      <c r="AH25" s="24"/>
+      <c r="AI25" s="24"/>
+      <c r="AJ25" s="24"/>
+      <c r="AK25" s="24"/>
+      <c r="AL25" s="24"/>
+      <c r="AM25" s="24"/>
+      <c r="AN25" s="24"/>
+      <c r="AO25" s="24"/>
+      <c r="AP25" s="24"/>
+      <c r="AQ25" s="24"/>
+      <c r="AR25" s="24"/>
+      <c r="AS25" s="24"/>
+      <c r="AT25" s="24"/>
+      <c r="AU25" s="24"/>
+      <c r="AV25" s="24"/>
+      <c r="AW25" s="24"/>
+      <c r="AX25" s="24"/>
+      <c r="AY25" s="24"/>
+      <c r="AZ25" s="24"/>
+      <c r="BA25" s="24"/>
+      <c r="BB25" s="24"/>
+      <c r="BC25" s="24"/>
+      <c r="BD25" s="24"/>
+      <c r="BE25" s="24"/>
+      <c r="BF25" s="24"/>
+      <c r="BG25" s="24"/>
+      <c r="BH25" s="24"/>
+      <c r="BI25" s="24"/>
+      <c r="BJ25" s="24"/>
+      <c r="BK25" s="24"/>
     </row>
     <row r="26" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="B26" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="34">
+      <c r="B26" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="32">
         <v>7</v>
       </c>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
-      <c r="Y26" s="26"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="26"/>
-      <c r="AD26" s="26"/>
-      <c r="AE26" s="26"/>
-      <c r="AF26" s="26"/>
-      <c r="AG26" s="26"/>
-      <c r="AH26" s="26"/>
-      <c r="AI26" s="26"/>
-      <c r="AJ26" s="26"/>
-      <c r="AK26" s="26"/>
-      <c r="AL26" s="26"/>
-      <c r="AM26" s="26"/>
-      <c r="AN26" s="26"/>
-      <c r="AO26" s="26"/>
-      <c r="AP26" s="26"/>
-      <c r="AQ26" s="26"/>
-      <c r="AR26" s="26"/>
-      <c r="AS26" s="26"/>
-      <c r="AT26" s="26"/>
-      <c r="AU26" s="26"/>
-      <c r="AV26" s="26"/>
-      <c r="AW26" s="26"/>
-      <c r="AX26" s="26"/>
-      <c r="AY26" s="26"/>
-      <c r="AZ26" s="26"/>
-      <c r="BA26" s="26"/>
-      <c r="BB26" s="26"/>
-      <c r="BC26" s="26"/>
-      <c r="BD26" s="26"/>
-      <c r="BE26" s="26"/>
-      <c r="BF26" s="26"/>
-      <c r="BG26" s="26"/>
-      <c r="BH26" s="26"/>
-      <c r="BI26" s="26"/>
-      <c r="BJ26" s="26"/>
-      <c r="BK26" s="26"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="24"/>
+      <c r="AH26" s="24"/>
+      <c r="AI26" s="24"/>
+      <c r="AJ26" s="24"/>
+      <c r="AK26" s="24"/>
+      <c r="AL26" s="24"/>
+      <c r="AM26" s="24"/>
+      <c r="AN26" s="24"/>
+      <c r="AO26" s="24"/>
+      <c r="AP26" s="24"/>
+      <c r="AQ26" s="24"/>
+      <c r="AR26" s="24"/>
+      <c r="AS26" s="24"/>
+      <c r="AT26" s="24"/>
+      <c r="AU26" s="24"/>
+      <c r="AV26" s="24"/>
+      <c r="AW26" s="24"/>
+      <c r="AX26" s="24"/>
+      <c r="AY26" s="24"/>
+      <c r="AZ26" s="24"/>
+      <c r="BA26" s="24"/>
+      <c r="BB26" s="24"/>
+      <c r="BC26" s="24"/>
+      <c r="BD26" s="24"/>
+      <c r="BE26" s="24"/>
+      <c r="BF26" s="24"/>
+      <c r="BG26" s="24"/>
+      <c r="BH26" s="24"/>
+      <c r="BI26" s="24"/>
+      <c r="BJ26" s="24"/>
+      <c r="BK26" s="24"/>
     </row>
     <row r="27" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="32">
         <v>5</v>
       </c>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="26"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="26"/>
-      <c r="AC27" s="26"/>
-      <c r="AD27" s="26"/>
-      <c r="AE27" s="26"/>
-      <c r="AF27" s="26"/>
-      <c r="AG27" s="26"/>
-      <c r="AH27" s="26"/>
-      <c r="AI27" s="26"/>
-      <c r="AJ27" s="26"/>
-      <c r="AK27" s="26"/>
-      <c r="AL27" s="26"/>
-      <c r="AM27" s="26"/>
-      <c r="AN27" s="26"/>
-      <c r="AO27" s="26"/>
-      <c r="AP27" s="26"/>
-      <c r="AQ27" s="26"/>
-      <c r="AR27" s="26"/>
-      <c r="AS27" s="26"/>
-      <c r="AT27" s="26"/>
-      <c r="AU27" s="26"/>
-      <c r="AV27" s="26"/>
-      <c r="AW27" s="26"/>
-      <c r="AX27" s="26"/>
-      <c r="AY27" s="26"/>
-      <c r="AZ27" s="26"/>
-      <c r="BA27" s="26"/>
-      <c r="BB27" s="26"/>
-      <c r="BC27" s="26"/>
-      <c r="BD27" s="26"/>
-      <c r="BE27" s="26"/>
-      <c r="BF27" s="26"/>
-      <c r="BG27" s="26"/>
-      <c r="BH27" s="26"/>
-      <c r="BI27" s="26"/>
-      <c r="BJ27" s="26"/>
-      <c r="BK27" s="26"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="24"/>
+      <c r="AB27" s="24"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="24"/>
+      <c r="AF27" s="24"/>
+      <c r="AG27" s="24"/>
+      <c r="AH27" s="24"/>
+      <c r="AI27" s="24"/>
+      <c r="AJ27" s="24"/>
+      <c r="AK27" s="24"/>
+      <c r="AL27" s="24"/>
+      <c r="AM27" s="24"/>
+      <c r="AN27" s="24"/>
+      <c r="AO27" s="24"/>
+      <c r="AP27" s="24"/>
+      <c r="AQ27" s="24"/>
+      <c r="AR27" s="24"/>
+      <c r="AS27" s="24"/>
+      <c r="AT27" s="24"/>
+      <c r="AU27" s="24"/>
+      <c r="AV27" s="24"/>
+      <c r="AW27" s="24"/>
+      <c r="AX27" s="24"/>
+      <c r="AY27" s="24"/>
+      <c r="AZ27" s="24"/>
+      <c r="BA27" s="24"/>
+      <c r="BB27" s="24"/>
+      <c r="BC27" s="24"/>
+      <c r="BD27" s="24"/>
+      <c r="BE27" s="24"/>
+      <c r="BF27" s="24"/>
+      <c r="BG27" s="24"/>
+      <c r="BH27" s="24"/>
+      <c r="BI27" s="24"/>
+      <c r="BJ27" s="24"/>
+      <c r="BK27" s="24"/>
     </row>
     <row r="28" spans="1:63" x14ac:dyDescent="0.2">
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="32">
         <v>5</v>
       </c>
     </row>
@@ -3554,6 +3584,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="D4:E4"/>
@@ -3564,16 +3604,6 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -3587,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,26 +3636,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="A1" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="34">
         <v>42065</v>
       </c>
     </row>
@@ -3639,10 +3669,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="72"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -3671,622 +3701,596 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+    <row r="5" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="102" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="101"/>
+      <c r="F5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="93" t="s">
+      <c r="C6" s="103"/>
+      <c r="D6" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="94"/>
-      <c r="F5" s="23" t="s">
+      <c r="E6" s="101"/>
+      <c r="F6" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G6" s="18">
         <v>1</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-    </row>
-    <row r="6" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
-        <v>2</v>
-      </c>
-      <c r="B6" s="25" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="93" t="s">
+      <c r="C7" s="103"/>
+      <c r="D7" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="94"/>
-      <c r="F6" s="23" t="s">
+      <c r="E7" s="101"/>
+      <c r="F7" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G7" s="18">
         <v>1</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="105"/>
+      <c r="F8" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="18">
+        <v>1</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18">
+        <v>1</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>5</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="103"/>
+      <c r="D9" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="105"/>
+      <c r="F9" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18">
+        <v>1</v>
+      </c>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="10" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>6</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="103"/>
+      <c r="D10" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="105"/>
+      <c r="F10" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19">
+        <v>1</v>
+      </c>
+      <c r="J10" s="18"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="55">
+        <v>7</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="103"/>
+      <c r="D11" s="106" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="107"/>
+      <c r="F11" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="56">
+        <v>1</v>
+      </c>
+      <c r="H11" s="56"/>
+      <c r="I11" s="55">
+        <v>1</v>
+      </c>
+      <c r="J11" s="56"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="57"/>
+    </row>
+    <row r="12" spans="1:14" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>8</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="103"/>
+      <c r="D12" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="101"/>
+      <c r="F12" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="18">
+        <v>5</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19">
+        <v>2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>2</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>9</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="99"/>
+      <c r="F13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="27">
+        <v>2</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27">
+        <v>2</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>10</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="99"/>
+      <c r="F14" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="27">
+        <v>8</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="26">
+        <v>2</v>
+      </c>
+      <c r="J14" s="27">
         <v>3</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="93" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="29"/>
+    </row>
+    <row r="15" spans="1:14" s="30" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>11</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="23" t="s">
+      <c r="E15" s="99"/>
+      <c r="F15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="27">
+        <v>10</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="29"/>
+    </row>
+    <row r="16" spans="1:14" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>12</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="99"/>
+      <c r="F16" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="19">
-        <v>1</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
-        <v>4</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="97" t="s">
+      <c r="G16" s="27">
+        <v>10</v>
+      </c>
+      <c r="H16" s="27">
+        <v>2</v>
+      </c>
+      <c r="I16" s="26">
+        <v>2</v>
+      </c>
+      <c r="J16" s="27">
+        <v>2</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>13</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="99"/>
+      <c r="F17" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="27">
+        <v>5</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="29"/>
+    </row>
+    <row r="18" spans="1:14" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>14</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19">
-        <v>1</v>
-      </c>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
-        <v>5</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="97" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="19">
-        <v>1</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
-        <v>6</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="97" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1</v>
-      </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="21">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="23"/>
-    </row>
-    <row r="11" spans="1:14" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57">
-        <v>7</v>
-      </c>
-      <c r="B11" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="100"/>
-      <c r="F11" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="58">
-        <v>1</v>
-      </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="57">
-        <v>1</v>
-      </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="59"/>
-    </row>
-    <row r="12" spans="1:14" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="94"/>
-      <c r="F12" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="19">
-        <v>5</v>
-      </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="21">
-        <v>2</v>
-      </c>
-      <c r="J12" s="19">
-        <v>2</v>
-      </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="23"/>
-    </row>
-    <row r="13" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
-        <v>9</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="92"/>
-      <c r="F13" s="31" t="s">
+      <c r="E18" s="99"/>
+      <c r="F18" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="27">
+        <v>12</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="29"/>
+    </row>
+    <row r="19" spans="1:14" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>15</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="99"/>
+      <c r="F19" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="27">
+        <v>12</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="29"/>
+    </row>
+    <row r="20" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>16</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="99"/>
+      <c r="F20" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="29">
-        <v>2</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29">
-        <v>2</v>
-      </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="31"/>
-    </row>
-    <row r="14" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
-        <v>10</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="92"/>
-      <c r="F14" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="29">
-        <v>8</v>
-      </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="28">
-        <v>2</v>
-      </c>
-      <c r="J14" s="29">
+      <c r="G20" s="27">
+        <v>12</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27">
         <v>3</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="31"/>
-    </row>
-    <row r="15" spans="1:14" s="32" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
-        <v>11</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="91" t="s">
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="29"/>
+    </row>
+    <row r="21" spans="1:14" s="115" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="72">
+        <v>17</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="114"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="22" spans="1:14" s="115" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="73"/>
+      <c r="B22" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="31" t="s">
+      <c r="E22" s="105"/>
+      <c r="F22" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="29">
-        <v>10</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="31"/>
-    </row>
-    <row r="16" spans="1:14" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="G22" s="116">
         <v>12</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="29">
-        <v>10</v>
-      </c>
-      <c r="H16" s="29">
-        <v>2</v>
-      </c>
-      <c r="I16" s="28">
-        <v>2</v>
-      </c>
-      <c r="J16" s="29">
-        <v>2</v>
-      </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="31"/>
-    </row>
-    <row r="17" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
-        <v>13</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="29">
-        <v>5</v>
-      </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="31"/>
-    </row>
-    <row r="18" spans="1:14" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
-        <v>14</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="91" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="29">
-        <v>12</v>
-      </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="31"/>
-    </row>
-    <row r="19" spans="1:14" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
-        <v>15</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="92"/>
-      <c r="F19" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="29">
-        <v>12</v>
-      </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="31"/>
-    </row>
-    <row r="20" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
-        <v>16</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="92"/>
-      <c r="F20" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="29">
-        <v>12</v>
-      </c>
-      <c r="H20" s="29"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29">
-        <v>3</v>
-      </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="31"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="66">
-        <v>1</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
-      <c r="B33" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="102"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
-      <c r="B34" s="10" t="s">
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="1:14" s="115" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="73"/>
+      <c r="B23" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
-      <c r="B35" s="10" t="s">
+      <c r="C23" s="23"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="1:14" s="115" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="73"/>
+      <c r="B24" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="106"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="67"/>
-      <c r="B36" s="10" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="73"/>
+      <c r="B25" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="67"/>
-      <c r="B37" s="10" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="73"/>
+      <c r="B26" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="102"/>
-      <c r="E37" s="103"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="67"/>
-      <c r="B38" s="10" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="95"/>
+      <c r="B27" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="101"/>
-      <c r="B39" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A32:A39"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E35"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
+  <mergeCells count="26">
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:C2"/>
@@ -4301,9 +4305,21 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E24"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D25:E27"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="F25:F27"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32:F33 F36:F39 F5:F20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21:F22 F5:F20 F25">
       <formula1>StatusList</formula1>
     </dataValidation>
   </dataValidations>
@@ -4322,38 +4338,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="36.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>151</v>
+        <v>132</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>150</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="112" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="112"/>
+      <c r="D2" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="108"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>152</v>
+        <v>134</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>151</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
@@ -4438,7 +4454,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update task SPRINT 4
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1112,6 +1112,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1130,62 +1139,74 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1232,113 +1253,92 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1570,11 +1570,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1571666624"/>
-        <c:axId val="-1571665536"/>
+        <c:axId val="-694708672"/>
+        <c:axId val="-694707584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1571666624"/>
+        <c:axId val="-694708672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1571665536"/>
+        <c:crossAx val="-694707584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1625,7 +1625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1571665536"/>
+        <c:axId val="-694707584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1677,7 +1677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1571666624"/>
+        <c:crossAx val="-694708672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,11 +2034,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1571654656"/>
-        <c:axId val="-1571655200"/>
+        <c:axId val="-694709760"/>
+        <c:axId val="-694703776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1571654656"/>
+        <c:axId val="-694709760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1571655200"/>
+        <c:crossAx val="-694703776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2089,7 +2089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1571655200"/>
+        <c:axId val="-694703776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,7 +2140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1571654656"/>
+        <c:crossAx val="-694709760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3982,18 +3982,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4021,11 +4021,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -4034,9 +4034,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -4054,10 +4054,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -4293,7 +4293,7 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="84" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="75" t="s">
@@ -4335,7 +4335,7 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="75" t="s">
         <v>71</v>
       </c>
@@ -4449,7 +4449,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="83">
+      <c r="A14" s="77">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -4469,7 +4469,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
@@ -4507,7 +4507,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -4545,7 +4545,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="84"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -4583,7 +4583,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="84"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -4621,7 +4621,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -4660,15 +4660,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -4679,6 +4670,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -4711,11 +4711,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -4724,9 +4724,9 @@
       </c>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -4789,10 +4789,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -4880,10 +4880,10 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="99"/>
       <c r="F5" s="27" t="s">
         <v>92</v>
       </c>
@@ -4918,10 +4918,10 @@
         <v>114</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="91"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="26" t="s">
         <v>92</v>
       </c>
@@ -4956,8 +4956,8 @@
         <v>115</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="26" t="s">
         <v>92</v>
       </c>
@@ -4992,10 +4992,10 @@
         <v>104</v>
       </c>
       <c r="C8" s="25"/>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="91"/>
+      <c r="E8" s="93"/>
       <c r="F8" s="26" t="s">
         <v>92</v>
       </c>
@@ -5018,10 +5018,10 @@
         <v>106</v>
       </c>
       <c r="C9" s="31"/>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="91"/>
       <c r="F9" s="33" t="s">
         <v>76</v>
       </c>
@@ -5044,10 +5044,10 @@
         <v>107</v>
       </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="95"/>
+      <c r="E10" s="91"/>
       <c r="F10" s="33" t="s">
         <v>76</v>
       </c>
@@ -5070,10 +5070,10 @@
         <v>108</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="95"/>
+      <c r="E11" s="91"/>
       <c r="F11" s="33" t="s">
         <v>76</v>
       </c>
@@ -5192,10 +5192,10 @@
         <v>110</v>
       </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="96" t="s">
+      <c r="D15" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="97"/>
+      <c r="E15" s="89"/>
       <c r="F15" s="26" t="s">
         <v>92</v>
       </c>
@@ -5268,8 +5268,8 @@
         <v>121</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="95"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="33"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -5288,10 +5288,10 @@
         <v>116</v>
       </c>
       <c r="C18" s="32"/>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="95"/>
+      <c r="E18" s="91"/>
       <c r="F18" s="33" t="s">
         <v>76</v>
       </c>
@@ -5326,10 +5326,10 @@
         <v>117</v>
       </c>
       <c r="C19" s="41"/>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="101"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="42" t="s">
         <v>66</v>
       </c>
@@ -5352,10 +5352,10 @@
         <v>118</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="90" t="s">
+      <c r="D20" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="91"/>
+      <c r="E20" s="93"/>
       <c r="F20" s="26" t="s">
         <v>92</v>
       </c>
@@ -5390,10 +5390,10 @@
         <v>112</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="95"/>
+      <c r="E21" s="91"/>
       <c r="F21" s="33" t="s">
         <v>76</v>
       </c>
@@ -5428,10 +5428,10 @@
         <v>113</v>
       </c>
       <c r="C22" s="25"/>
-      <c r="D22" s="90" t="s">
+      <c r="D22" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="91"/>
+      <c r="E22" s="93"/>
       <c r="F22" s="26" t="s">
         <v>92</v>
       </c>
@@ -5466,10 +5466,10 @@
         <v>119</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="99"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="26" t="s">
         <v>92</v>
       </c>
@@ -5736,6 +5736,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D21:E21"/>
@@ -5746,16 +5756,6 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -5771,8 +5771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5790,11 +5790,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="18" t="s">
         <v>59</v>
       </c>
@@ -5803,9 +5803,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="18" t="s">
         <v>60</v>
       </c>
@@ -5862,13 +5862,13 @@
       <c r="B5" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="91"/>
       <c r="F5" s="33" t="s">
         <v>76</v>
       </c>
@@ -5890,11 +5890,11 @@
       <c r="B6" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="94" t="s">
+      <c r="C6" s="107"/>
+      <c r="D6" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="95"/>
+      <c r="E6" s="91"/>
       <c r="F6" s="33" t="s">
         <v>76</v>
       </c>
@@ -5916,11 +5916,11 @@
       <c r="B7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="94" t="s">
+      <c r="C7" s="107"/>
+      <c r="D7" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="91"/>
       <c r="F7" s="33" t="s">
         <v>76</v>
       </c>
@@ -5942,11 +5942,11 @@
       <c r="B8" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="122"/>
-      <c r="D8" s="96" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="97"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="26" t="s">
         <v>92</v>
       </c>
@@ -5982,11 +5982,11 @@
       <c r="B9" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="122"/>
-      <c r="D9" s="96" t="s">
+      <c r="C9" s="107"/>
+      <c r="D9" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="97"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="26" t="s">
         <v>92</v>
       </c>
@@ -6022,11 +6022,11 @@
       <c r="B10" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="122"/>
-      <c r="D10" s="96" t="s">
+      <c r="C10" s="107"/>
+      <c r="D10" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="97"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="26" t="s">
         <v>92</v>
       </c>
@@ -6062,11 +6062,11 @@
       <c r="B11" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="122"/>
-      <c r="D11" s="90" t="s">
+      <c r="C11" s="107"/>
+      <c r="D11" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="91"/>
+      <c r="E11" s="93"/>
       <c r="F11" s="26" t="s">
         <v>92</v>
       </c>
@@ -6102,11 +6102,11 @@
       <c r="B12" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="122"/>
-      <c r="D12" s="90" t="s">
+      <c r="C12" s="107"/>
+      <c r="D12" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="91"/>
+      <c r="E12" s="93"/>
       <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
@@ -6142,11 +6142,11 @@
       <c r="B13" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="98" t="s">
+      <c r="C13" s="108"/>
+      <c r="D13" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="99"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="26" t="s">
         <v>92</v>
       </c>
@@ -6183,10 +6183,10 @@
         <v>140</v>
       </c>
       <c r="C14" s="25"/>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="99"/>
+      <c r="E14" s="95"/>
       <c r="F14" s="26" t="s">
         <v>92</v>
       </c>
@@ -6225,10 +6225,10 @@
       <c r="C15" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="117" t="s">
+      <c r="D15" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="118"/>
+      <c r="E15" s="103"/>
       <c r="F15" s="33" t="s">
         <v>76</v>
       </c>
@@ -6253,10 +6253,10 @@
       <c r="C16" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="95"/>
       <c r="F16" s="26" t="s">
         <v>92</v>
       </c>
@@ -6293,10 +6293,10 @@
         <v>138</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="117" t="s">
+      <c r="D17" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="118"/>
+      <c r="E17" s="103"/>
       <c r="F17" s="33" t="s">
         <v>76</v>
       </c>
@@ -6335,10 +6335,10 @@
       <c r="C18" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="99"/>
+      <c r="E18" s="95"/>
       <c r="F18" s="26" t="s">
         <v>92</v>
       </c>
@@ -6377,10 +6377,10 @@
       <c r="C19" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="99"/>
+      <c r="E19" s="95"/>
       <c r="F19" s="26" t="s">
         <v>92</v>
       </c>
@@ -6417,10 +6417,10 @@
         <v>144</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="99"/>
+      <c r="E20" s="95"/>
       <c r="F20" s="26" t="s">
         <v>92</v>
       </c>
@@ -6457,10 +6457,10 @@
         <v>149</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="26" t="s">
         <v>92</v>
       </c>
@@ -6490,15 +6490,15 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="108">
+      <c r="A22" s="115">
         <v>18</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="32"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="112"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="119"/>
       <c r="F22" s="31"/>
       <c r="G22" s="59"/>
       <c r="H22" s="31"/>
@@ -6510,7 +6510,7 @@
       <c r="N22" s="59"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
+      <c r="A23" s="116"/>
       <c r="B23" s="31" t="s">
         <v>98</v>
       </c>
@@ -6519,10 +6519,10 @@
         <v>68</v>
       </c>
       <c r="E23" s="87"/>
-      <c r="F23" s="102" t="s">
+      <c r="F23" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="105">
+      <c r="G23" s="112">
         <v>12</v>
       </c>
       <c r="H23" s="31"/>
@@ -6534,15 +6534,15 @@
       <c r="N23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
+      <c r="A24" s="116"/>
       <c r="B24" s="31" t="s">
         <v>99</v>
       </c>
       <c r="C24" s="32"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="106"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="113"/>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -6552,15 +6552,15 @@
       <c r="N24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="31" t="s">
         <v>100</v>
       </c>
       <c r="C25" s="32"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="107"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="114"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -6672,6 +6672,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:C2"/>
@@ -6685,17 +6696,6 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="C5:C13"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -6712,8 +6712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6731,11 +6731,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -6744,9 +6744,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -6764,10 +6764,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -6803,13 +6803,13 @@
       <c r="B5" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="149" t="s">
+      <c r="C5" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="124" t="s">
+      <c r="D5" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="125"/>
+      <c r="E5" s="152"/>
       <c r="F5" s="46" t="s">
         <v>76</v>
       </c>
@@ -6831,11 +6831,11 @@
       <c r="B6" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="124" t="s">
+      <c r="C6" s="131"/>
+      <c r="D6" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="125"/>
+      <c r="E6" s="152"/>
       <c r="F6" s="46" t="s">
         <v>76</v>
       </c>
@@ -6857,11 +6857,11 @@
       <c r="B7" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="150"/>
-      <c r="D7" s="124" t="s">
+      <c r="C7" s="131"/>
+      <c r="D7" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="125"/>
+      <c r="E7" s="152"/>
       <c r="F7" s="46" t="s">
         <v>76</v>
       </c>
@@ -6884,10 +6884,10 @@
         <v>163</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="152"/>
+      <c r="E8" s="133"/>
       <c r="F8" s="68" t="s">
         <v>66</v>
       </c>
@@ -6910,10 +6910,10 @@
         <v>165</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="151" t="s">
+      <c r="D9" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="152"/>
+      <c r="E9" s="133"/>
       <c r="F9" s="68" t="s">
         <v>66</v>
       </c>
@@ -6936,10 +6936,10 @@
         <v>164</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="151" t="s">
+      <c r="D10" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="152"/>
+      <c r="E10" s="133"/>
       <c r="F10" s="68" t="s">
         <v>66</v>
       </c>
@@ -6962,10 +6962,10 @@
         <v>166</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="137" t="s">
+      <c r="D11" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="138"/>
+      <c r="E11" s="135"/>
       <c r="F11" s="68" t="s">
         <v>66</v>
       </c>
@@ -6988,10 +6988,10 @@
         <v>168</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="137" t="s">
+      <c r="D12" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="138"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="68" t="s">
         <v>66</v>
       </c>
@@ -7014,10 +7014,10 @@
         <v>167</v>
       </c>
       <c r="C13" s="67"/>
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="148"/>
       <c r="F13" s="68" t="s">
         <v>66</v>
       </c>
@@ -7040,10 +7040,10 @@
         <v>169</v>
       </c>
       <c r="C14" s="67"/>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="147" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="148"/>
       <c r="F14" s="68" t="s">
         <v>66</v>
       </c>
@@ -7066,10 +7066,10 @@
         <v>170</v>
       </c>
       <c r="C15" s="72"/>
-      <c r="D15" s="139" t="s">
+      <c r="D15" s="147" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="140"/>
+      <c r="E15" s="148"/>
       <c r="F15" s="68" t="s">
         <v>66</v>
       </c>
@@ -7094,10 +7094,10 @@
       <c r="C16" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="141" t="s">
+      <c r="D16" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="150"/>
       <c r="F16" s="46" t="s">
         <v>76</v>
       </c>
@@ -7120,10 +7120,10 @@
         <v>138</v>
       </c>
       <c r="C17" s="45"/>
-      <c r="D17" s="141" t="s">
+      <c r="D17" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="142"/>
+      <c r="E17" s="150"/>
       <c r="F17" s="46" t="s">
         <v>76</v>
       </c>
@@ -7153,15 +7153,15 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="126">
+      <c r="A18" s="136">
         <v>14</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="45"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="130"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
       <c r="F18" s="47"/>
       <c r="G18" s="48"/>
       <c r="H18" s="47"/>
@@ -7173,19 +7173,19 @@
       <c r="N18" s="48"/>
     </row>
     <row r="19" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="127"/>
+      <c r="A19" s="137"/>
       <c r="B19" s="45" t="s">
         <v>98</v>
       </c>
       <c r="C19" s="45"/>
-      <c r="D19" s="131" t="s">
+      <c r="D19" s="141" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="132"/>
-      <c r="F19" s="143" t="s">
+      <c r="E19" s="142"/>
+      <c r="F19" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="146">
+      <c r="G19" s="127">
         <v>12</v>
       </c>
       <c r="H19" s="47"/>
@@ -7197,15 +7197,15 @@
       <c r="N19" s="48"/>
     </row>
     <row r="20" spans="1:14" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="127"/>
+      <c r="A20" s="137"/>
       <c r="B20" s="45" t="s">
         <v>99</v>
       </c>
       <c r="C20" s="45"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="147"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="128"/>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
@@ -7215,15 +7215,15 @@
       <c r="N20" s="48"/>
     </row>
     <row r="21" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="128"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="45" t="s">
         <v>100</v>
       </c>
       <c r="C21" s="45"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="145"/>
-      <c r="G21" s="148"/>
+      <c r="D21" s="145"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="129"/>
       <c r="H21" s="47"/>
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
@@ -7280,13 +7280,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E21"/>
@@ -7296,11 +7294,13 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">

</xml_diff>

<commit_message>
Add CategoryManagement Page for Admin
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="StatusList">Refrence!$A$1:$A$4</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1112,6 +1112,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1130,62 +1139,74 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1232,113 +1253,92 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1549,11 +1549,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="90902912"/>
-        <c:axId val="90905600"/>
+        <c:axId val="99136256"/>
+        <c:axId val="99138944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90902912"/>
+        <c:axId val="99136256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90905600"/>
+        <c:crossAx val="99138944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1604,7 +1604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90905600"/>
+        <c:axId val="99138944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1656,7 +1656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90902912"/>
+        <c:crossAx val="99136256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1992,11 +1992,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="90939776"/>
-        <c:axId val="90941312"/>
+        <c:axId val="160015104"/>
+        <c:axId val="160016640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90939776"/>
+        <c:axId val="160015104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,7 +2039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90941312"/>
+        <c:crossAx val="160016640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2047,7 +2047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90941312"/>
+        <c:axId val="160016640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90939776"/>
+        <c:crossAx val="160015104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3939,18 +3939,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3978,11 +3978,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -3991,9 +3991,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -4011,10 +4011,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -4250,7 +4250,7 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="84" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="75" t="s">
@@ -4292,7 +4292,7 @@
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="75" t="s">
         <v>71</v>
       </c>
@@ -4406,7 +4406,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="83">
+      <c r="A14" s="77">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -4426,7 +4426,7 @@
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="13" t="s">
         <v>88</v>
       </c>
@@ -4464,7 +4464,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="13" t="s">
         <v>89</v>
       </c>
@@ -4502,7 +4502,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="84"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="13" t="s">
         <v>90</v>
       </c>
@@ -4540,7 +4540,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="84"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="13" t="s">
         <v>91</v>
       </c>
@@ -4578,7 +4578,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="14" t="s">
         <v>93</v>
       </c>
@@ -4617,15 +4617,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
@@ -4636,6 +4627,15 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">
@@ -4668,11 +4668,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -4681,9 +4681,9 @@
       </c>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -4746,10 +4746,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -4837,10 +4837,10 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="99"/>
       <c r="F5" s="27" t="s">
         <v>92</v>
       </c>
@@ -4875,10 +4875,10 @@
         <v>114</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="91"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="26" t="s">
         <v>92</v>
       </c>
@@ -4913,8 +4913,8 @@
         <v>115</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="26" t="s">
         <v>92</v>
       </c>
@@ -4949,10 +4949,10 @@
         <v>104</v>
       </c>
       <c r="C8" s="25"/>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="91"/>
+      <c r="E8" s="93"/>
       <c r="F8" s="26" t="s">
         <v>92</v>
       </c>
@@ -4975,10 +4975,10 @@
         <v>106</v>
       </c>
       <c r="C9" s="31"/>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="91"/>
       <c r="F9" s="33" t="s">
         <v>76</v>
       </c>
@@ -5001,10 +5001,10 @@
         <v>107</v>
       </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="95"/>
+      <c r="E10" s="91"/>
       <c r="F10" s="33" t="s">
         <v>76</v>
       </c>
@@ -5027,10 +5027,10 @@
         <v>108</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="95"/>
+      <c r="E11" s="91"/>
       <c r="F11" s="33" t="s">
         <v>76</v>
       </c>
@@ -5149,10 +5149,10 @@
         <v>110</v>
       </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="96" t="s">
+      <c r="D15" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="97"/>
+      <c r="E15" s="89"/>
       <c r="F15" s="26" t="s">
         <v>92</v>
       </c>
@@ -5225,8 +5225,8 @@
         <v>121</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="95"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="33"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -5245,10 +5245,10 @@
         <v>116</v>
       </c>
       <c r="C18" s="32"/>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="95"/>
+      <c r="E18" s="91"/>
       <c r="F18" s="33" t="s">
         <v>76</v>
       </c>
@@ -5283,10 +5283,10 @@
         <v>117</v>
       </c>
       <c r="C19" s="41"/>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="101"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="42" t="s">
         <v>66</v>
       </c>
@@ -5309,10 +5309,10 @@
         <v>118</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="90" t="s">
+      <c r="D20" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="91"/>
+      <c r="E20" s="93"/>
       <c r="F20" s="26" t="s">
         <v>92</v>
       </c>
@@ -5347,10 +5347,10 @@
         <v>112</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="95"/>
+      <c r="E21" s="91"/>
       <c r="F21" s="33" t="s">
         <v>76</v>
       </c>
@@ -5385,10 +5385,10 @@
         <v>113</v>
       </c>
       <c r="C22" s="25"/>
-      <c r="D22" s="90" t="s">
+      <c r="D22" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="91"/>
+      <c r="E22" s="93"/>
       <c r="F22" s="26" t="s">
         <v>92</v>
       </c>
@@ -5423,10 +5423,10 @@
         <v>119</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="99"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="26" t="s">
         <v>92</v>
       </c>
@@ -5693,6 +5693,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D21:E21"/>
@@ -5703,16 +5713,6 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -5747,11 +5747,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="18" t="s">
         <v>59</v>
       </c>
@@ -5760,9 +5760,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="120"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="18" t="s">
         <v>60</v>
       </c>
@@ -5819,13 +5819,13 @@
       <c r="B5" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="106" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="D5" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="91"/>
       <c r="F5" s="33" t="s">
         <v>76</v>
       </c>
@@ -5847,11 +5847,11 @@
       <c r="B6" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="94" t="s">
+      <c r="C6" s="107"/>
+      <c r="D6" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="95"/>
+      <c r="E6" s="91"/>
       <c r="F6" s="33" t="s">
         <v>76</v>
       </c>
@@ -5873,11 +5873,11 @@
       <c r="B7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="94" t="s">
+      <c r="C7" s="107"/>
+      <c r="D7" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="91"/>
       <c r="F7" s="33" t="s">
         <v>76</v>
       </c>
@@ -5899,11 +5899,11 @@
       <c r="B8" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="122"/>
-      <c r="D8" s="96" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="97"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="26" t="s">
         <v>92</v>
       </c>
@@ -5939,11 +5939,11 @@
       <c r="B9" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="122"/>
-      <c r="D9" s="96" t="s">
+      <c r="C9" s="107"/>
+      <c r="D9" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="97"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="26" t="s">
         <v>92</v>
       </c>
@@ -5979,11 +5979,11 @@
       <c r="B10" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="122"/>
-      <c r="D10" s="96" t="s">
+      <c r="C10" s="107"/>
+      <c r="D10" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="97"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="26" t="s">
         <v>92</v>
       </c>
@@ -6019,11 +6019,11 @@
       <c r="B11" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="122"/>
-      <c r="D11" s="90" t="s">
+      <c r="C11" s="107"/>
+      <c r="D11" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="91"/>
+      <c r="E11" s="93"/>
       <c r="F11" s="26" t="s">
         <v>92</v>
       </c>
@@ -6059,11 +6059,11 @@
       <c r="B12" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="122"/>
-      <c r="D12" s="90" t="s">
+      <c r="C12" s="107"/>
+      <c r="D12" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="91"/>
+      <c r="E12" s="93"/>
       <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
@@ -6099,11 +6099,11 @@
       <c r="B13" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="98" t="s">
+      <c r="C13" s="108"/>
+      <c r="D13" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="99"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="26" t="s">
         <v>92</v>
       </c>
@@ -6140,10 +6140,10 @@
         <v>140</v>
       </c>
       <c r="C14" s="25"/>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="99"/>
+      <c r="E14" s="95"/>
       <c r="F14" s="26" t="s">
         <v>92</v>
       </c>
@@ -6182,10 +6182,10 @@
       <c r="C15" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="117" t="s">
+      <c r="D15" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="118"/>
+      <c r="E15" s="103"/>
       <c r="F15" s="33" t="s">
         <v>76</v>
       </c>
@@ -6210,10 +6210,10 @@
       <c r="C16" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="95"/>
       <c r="F16" s="26" t="s">
         <v>92</v>
       </c>
@@ -6250,10 +6250,10 @@
         <v>138</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="117" t="s">
+      <c r="D17" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="118"/>
+      <c r="E17" s="103"/>
       <c r="F17" s="33" t="s">
         <v>76</v>
       </c>
@@ -6292,10 +6292,10 @@
       <c r="C18" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="99"/>
+      <c r="E18" s="95"/>
       <c r="F18" s="26" t="s">
         <v>92</v>
       </c>
@@ -6334,10 +6334,10 @@
       <c r="C19" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="99"/>
+      <c r="E19" s="95"/>
       <c r="F19" s="26" t="s">
         <v>92</v>
       </c>
@@ -6374,10 +6374,10 @@
         <v>144</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="99"/>
+      <c r="E20" s="95"/>
       <c r="F20" s="26" t="s">
         <v>92</v>
       </c>
@@ -6414,10 +6414,10 @@
         <v>149</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="26" t="s">
         <v>92</v>
       </c>
@@ -6447,15 +6447,15 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="108">
+      <c r="A22" s="115">
         <v>18</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="32"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="112"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="119"/>
       <c r="F22" s="31"/>
       <c r="G22" s="59"/>
       <c r="H22" s="31"/>
@@ -6467,7 +6467,7 @@
       <c r="N22" s="59"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
+      <c r="A23" s="116"/>
       <c r="B23" s="31" t="s">
         <v>98</v>
       </c>
@@ -6476,10 +6476,10 @@
         <v>68</v>
       </c>
       <c r="E23" s="87"/>
-      <c r="F23" s="102" t="s">
+      <c r="F23" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="105">
+      <c r="G23" s="112">
         <v>12</v>
       </c>
       <c r="H23" s="31"/>
@@ -6491,15 +6491,15 @@
       <c r="N23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
+      <c r="A24" s="116"/>
       <c r="B24" s="31" t="s">
         <v>99</v>
       </c>
       <c r="C24" s="32"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="106"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="113"/>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -6509,15 +6509,15 @@
       <c r="N24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
+      <c r="A25" s="117"/>
       <c r="B25" s="31" t="s">
         <v>100</v>
       </c>
       <c r="C25" s="32"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="107"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="114"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -6629,6 +6629,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:C2"/>
@@ -6642,17 +6653,6 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="C5:C13"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F23">
@@ -6669,8 +6669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6688,11 +6688,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
@@ -6701,9 +6701,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
@@ -6721,10 +6721,10 @@
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="83"/>
       <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
@@ -6760,13 +6760,13 @@
       <c r="B5" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="149" t="s">
+      <c r="C5" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="124" t="s">
+      <c r="D5" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="125"/>
+      <c r="E5" s="152"/>
       <c r="F5" s="46" t="s">
         <v>76</v>
       </c>
@@ -6788,11 +6788,11 @@
       <c r="B6" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="124" t="s">
+      <c r="C6" s="131"/>
+      <c r="D6" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="125"/>
+      <c r="E6" s="152"/>
       <c r="F6" s="46" t="s">
         <v>76</v>
       </c>
@@ -6814,11 +6814,11 @@
       <c r="B7" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="150"/>
-      <c r="D7" s="124" t="s">
+      <c r="C7" s="131"/>
+      <c r="D7" s="151" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="125"/>
+      <c r="E7" s="152"/>
       <c r="F7" s="46" t="s">
         <v>76</v>
       </c>
@@ -6841,10 +6841,10 @@
         <v>163</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="152"/>
+      <c r="E8" s="133"/>
       <c r="F8" s="68" t="s">
         <v>66</v>
       </c>
@@ -6867,10 +6867,10 @@
         <v>165</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="151" t="s">
+      <c r="D9" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="152"/>
+      <c r="E9" s="133"/>
       <c r="F9" s="68" t="s">
         <v>66</v>
       </c>
@@ -6893,10 +6893,10 @@
         <v>164</v>
       </c>
       <c r="C10" s="67"/>
-      <c r="D10" s="151" t="s">
+      <c r="D10" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="152"/>
+      <c r="E10" s="133"/>
       <c r="F10" s="68" t="s">
         <v>66</v>
       </c>
@@ -6919,10 +6919,10 @@
         <v>166</v>
       </c>
       <c r="C11" s="67"/>
-      <c r="D11" s="137" t="s">
+      <c r="D11" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="138"/>
+      <c r="E11" s="135"/>
       <c r="F11" s="68" t="s">
         <v>66</v>
       </c>
@@ -6945,10 +6945,10 @@
         <v>168</v>
       </c>
       <c r="C12" s="67"/>
-      <c r="D12" s="137" t="s">
+      <c r="D12" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="138"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="68" t="s">
         <v>66</v>
       </c>
@@ -6971,10 +6971,10 @@
         <v>167</v>
       </c>
       <c r="C13" s="67"/>
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="148"/>
       <c r="F13" s="68" t="s">
         <v>66</v>
       </c>
@@ -6997,10 +6997,10 @@
         <v>169</v>
       </c>
       <c r="C14" s="67"/>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="147" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="148"/>
       <c r="F14" s="68" t="s">
         <v>66</v>
       </c>
@@ -7023,10 +7023,10 @@
         <v>170</v>
       </c>
       <c r="C15" s="72"/>
-      <c r="D15" s="139" t="s">
+      <c r="D15" s="147" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="140"/>
+      <c r="E15" s="148"/>
       <c r="F15" s="68" t="s">
         <v>76</v>
       </c>
@@ -7034,8 +7034,12 @@
         <v>10</v>
       </c>
       <c r="H15" s="67"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="67"/>
+      <c r="I15" s="65">
+        <v>2</v>
+      </c>
+      <c r="J15" s="67">
+        <v>2</v>
+      </c>
       <c r="K15" s="72"/>
       <c r="L15" s="72"/>
       <c r="M15" s="67"/>
@@ -7051,10 +7055,10 @@
       <c r="C16" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="141" t="s">
+      <c r="D16" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="150"/>
       <c r="F16" s="46" t="s">
         <v>76</v>
       </c>
@@ -7077,10 +7081,10 @@
         <v>138</v>
       </c>
       <c r="C17" s="45"/>
-      <c r="D17" s="141" t="s">
+      <c r="D17" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="142"/>
+      <c r="E17" s="150"/>
       <c r="F17" s="46" t="s">
         <v>76</v>
       </c>
@@ -7110,15 +7114,15 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="126">
+      <c r="A18" s="136">
         <v>14</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="45"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="130"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="140"/>
       <c r="F18" s="47"/>
       <c r="G18" s="48"/>
       <c r="H18" s="47"/>
@@ -7130,19 +7134,19 @@
       <c r="N18" s="48"/>
     </row>
     <row r="19" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="127"/>
+      <c r="A19" s="137"/>
       <c r="B19" s="45" t="s">
         <v>98</v>
       </c>
       <c r="C19" s="45"/>
-      <c r="D19" s="131" t="s">
+      <c r="D19" s="141" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="132"/>
-      <c r="F19" s="143" t="s">
+      <c r="E19" s="142"/>
+      <c r="F19" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="146">
+      <c r="G19" s="127">
         <v>12</v>
       </c>
       <c r="H19" s="47"/>
@@ -7154,15 +7158,15 @@
       <c r="N19" s="48"/>
     </row>
     <row r="20" spans="1:14" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="127"/>
+      <c r="A20" s="137"/>
       <c r="B20" s="45" t="s">
         <v>99</v>
       </c>
       <c r="C20" s="45"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="147"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="128"/>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
@@ -7172,15 +7176,15 @@
       <c r="N20" s="48"/>
     </row>
     <row r="21" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="128"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="45" t="s">
         <v>100</v>
       </c>
       <c r="C21" s="45"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="145"/>
-      <c r="G21" s="148"/>
+      <c r="D21" s="145"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="129"/>
       <c r="H21" s="47"/>
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
@@ -7237,13 +7241,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E21"/>
@@ -7253,11 +7255,13 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F19">

</xml_diff>